<commit_message>
New Data Model and Desc, Example file
- Added new Desc and Example Tables CSV file and New Data Model
</commit_message>
<xml_diff>
--- a/docs/Desc and Example Tables.xlsx
+++ b/docs/Desc and Example Tables.xlsx
@@ -8,19 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17737\Desktop\FPT\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0B0016E-C7CF-48F9-B0BB-CB8D40A38CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926A63C4-662C-4881-832A-4BF20C39C4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="7" xr2:uid="{76F2D5F5-96DF-42B7-9620-589D1FA50423}"/>
+    <workbookView xWindow="-28800" yWindow="15" windowWidth="28800" windowHeight="16185" activeTab="3" xr2:uid="{76F2D5F5-96DF-42B7-9620-589D1FA50423}"/>
   </bookViews>
   <sheets>
     <sheet name="Insurance" sheetId="2" r:id="rId1"/>
-    <sheet name="Demographic" sheetId="3" r:id="rId2"/>
-    <sheet name="Patient" sheetId="4" r:id="rId3"/>
-    <sheet name="Disease" sheetId="5" r:id="rId4"/>
-    <sheet name="Symptom" sheetId="6" r:id="rId5"/>
-    <sheet name="Diagnosis" sheetId="7" r:id="rId6"/>
-    <sheet name="Date" sheetId="8" r:id="rId7"/>
-    <sheet name="Medical" sheetId="1" r:id="rId8"/>
+    <sheet name="Patient" sheetId="4" r:id="rId2"/>
+    <sheet name="Disease" sheetId="5" r:id="rId3"/>
+    <sheet name="Symptom" sheetId="6" r:id="rId4"/>
+    <sheet name="Diagnosis" sheetId="7" r:id="rId5"/>
+    <sheet name="Medical" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="225">
   <si>
     <t>Medical_ID</t>
   </si>
@@ -55,12 +53,6 @@
     <t>Date_ID</t>
   </si>
   <si>
-    <t>Appointment_Start_Date</t>
-  </si>
-  <si>
-    <t>Appointment_End_Date</t>
-  </si>
-  <si>
     <t>Insurance_Number</t>
   </si>
   <si>
@@ -91,9 +83,6 @@
     <t>datetime</t>
   </si>
   <si>
-    <t>varchar(3)</t>
-  </si>
-  <si>
     <t>Blood_Sugar_mgdL</t>
   </si>
   <si>
@@ -520,9 +509,6 @@
     <t>O</t>
   </si>
   <si>
-    <t>Demographic_ID</t>
-  </si>
-  <si>
     <t>Insurance_ID</t>
   </si>
   <si>
@@ -535,238 +521,199 @@
     <t>P1-&gt;P1000</t>
   </si>
   <si>
-    <t>2 types(HMO, PPO)</t>
+    <t>I2000-I3000</t>
+  </si>
+  <si>
+    <t>I2000</t>
+  </si>
+  <si>
+    <t>I2001</t>
+  </si>
+  <si>
+    <t>I2002</t>
+  </si>
+  <si>
+    <t>I2003</t>
+  </si>
+  <si>
+    <t>HMO</t>
+  </si>
+  <si>
+    <t>Insurance_Cover_Ammount</t>
+  </si>
+  <si>
+    <t>random (6000, 9000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>random (HMO. PPO)</t>
+  </si>
+  <si>
+    <t>giống với bảng Demographic</t>
+  </si>
+  <si>
+    <t>PMO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1/4/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10/5/2024</t>
+  </si>
+  <si>
+    <t>Matching HMO = 6k, PMO = 9k</t>
+  </si>
+  <si>
+    <t>DA1-DA5000</t>
+  </si>
+  <si>
+    <t>(S1-S32)</t>
+  </si>
+  <si>
+    <t>random(S1-S32)</t>
+  </si>
+  <si>
+    <t>DA1</t>
+  </si>
+  <si>
+    <t>DA2</t>
+  </si>
+  <si>
+    <t>DA3</t>
+  </si>
+  <si>
+    <t>DA4</t>
+  </si>
+  <si>
+    <t>DA5</t>
+  </si>
+  <si>
+    <t>DA6</t>
+  </si>
+  <si>
+    <t>DA7</t>
+  </si>
+  <si>
+    <t>DA8</t>
+  </si>
+  <si>
+    <t>M1-M5000</t>
+  </si>
+  <si>
+    <t>random DA1-5000</t>
+  </si>
+  <si>
+    <t>random P1-P1000 (5000 lần)</t>
+  </si>
+  <si>
+    <t>random (I2000-I3000)</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>M5</t>
+  </si>
+  <si>
+    <t>M6</t>
+  </si>
+  <si>
+    <t>Total: 5k columns</t>
+  </si>
+  <si>
+    <t>DT1</t>
+  </si>
+  <si>
+    <t>DT2</t>
+  </si>
+  <si>
+    <t>DT3</t>
+  </si>
+  <si>
+    <t>DT4</t>
+  </si>
+  <si>
+    <t>DT5</t>
+  </si>
+  <si>
+    <t>DT6</t>
+  </si>
+  <si>
+    <t>I2004</t>
+  </si>
+  <si>
+    <t>I2005</t>
+  </si>
+  <si>
+    <t>Theo bảng Patient(base on P_ID)</t>
+  </si>
+  <si>
+    <t>Column9</t>
+  </si>
+  <si>
+    <t>Column10</t>
+  </si>
+  <si>
+    <t>Column11</t>
+  </si>
+  <si>
+    <t>Column12</t>
+  </si>
+  <si>
+    <t>Total: 5000 colums</t>
+  </si>
+  <si>
+    <t>Total: 32 columns</t>
+  </si>
+  <si>
+    <t>Total: 5 colums</t>
+  </si>
+  <si>
+    <t>Total: 1000 columns</t>
+  </si>
+  <si>
+    <t>Symptom_ID</t>
+  </si>
+  <si>
+    <t>Symptom_Name</t>
+  </si>
+  <si>
+    <t>Symptom_Stage</t>
+  </si>
+  <si>
+    <t>Symptom_Stage_Desc</t>
+  </si>
+  <si>
+    <t>Symptom_Repeated_Time</t>
+  </si>
+  <si>
+    <t>random(1, 0)</t>
+  </si>
+  <si>
+    <t>Random (I2000-I3000)</t>
+  </si>
+  <si>
+    <t>I2I20</t>
+  </si>
+  <si>
+    <t>Appointment_Date</t>
   </si>
   <si>
     <t>date</t>
   </si>
   <si>
-    <t>P1-P1000</t>
-  </si>
-  <si>
-    <t>I2000-I3000</t>
-  </si>
-  <si>
-    <t>I2000</t>
-  </si>
-  <si>
-    <t>I2001</t>
-  </si>
-  <si>
-    <t>I2002</t>
-  </si>
-  <si>
-    <t>I2003</t>
-  </si>
-  <si>
-    <t>HMO</t>
-  </si>
-  <si>
-    <t>PPO</t>
-  </si>
-  <si>
-    <t>Insurance_Cover_Ammount</t>
-  </si>
-  <si>
-    <t>random (6000, 9000)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>random (HMO. PPO)</t>
-  </si>
-  <si>
-    <t>giống với bảng Demographic</t>
-  </si>
-  <si>
-    <t>PMO</t>
-  </si>
-  <si>
-    <t>Random 3 types (1/4/2025, 1/4/2023/, 10/5/2024)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1/4/2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10/5/2024</t>
-  </si>
-  <si>
-    <t>Matching HMO = 6k, PMO = 9k</t>
-  </si>
-  <si>
-    <t>DG1-DG1000</t>
-  </si>
-  <si>
-    <t>DA1-DA5000</t>
-  </si>
-  <si>
-    <t>(S1-S32)</t>
-  </si>
-  <si>
-    <t>random(S1-S32)</t>
-  </si>
-  <si>
-    <t>DA1</t>
-  </si>
-  <si>
-    <t>DA2</t>
-  </si>
-  <si>
-    <t>DA3</t>
-  </si>
-  <si>
-    <t>DA4</t>
-  </si>
-  <si>
-    <t>DA5</t>
-  </si>
-  <si>
-    <t>DA6</t>
-  </si>
-  <si>
-    <t>DA7</t>
-  </si>
-  <si>
-    <t>DA8</t>
-  </si>
-  <si>
-    <t>DT1-DT5000</t>
-  </si>
-  <si>
-    <t>Random date (year=2021)</t>
-  </si>
-  <si>
-    <t>Random date (year=2020)</t>
-  </si>
-  <si>
-    <t>M1-M5000</t>
-  </si>
-  <si>
-    <t>random DA1-5000</t>
-  </si>
-  <si>
-    <t>random P1-P1000 (5000 lần)</t>
-  </si>
-  <si>
-    <t>theo bảng Date</t>
-  </si>
-  <si>
-    <t>random (I2000-I3000)</t>
-  </si>
-  <si>
-    <t>Column5</t>
-  </si>
-  <si>
-    <t>M1</t>
-  </si>
-  <si>
-    <t>M2</t>
-  </si>
-  <si>
-    <t>M3</t>
-  </si>
-  <si>
-    <t>M4</t>
-  </si>
-  <si>
-    <t>M5</t>
-  </si>
-  <si>
-    <t>M6</t>
-  </si>
-  <si>
-    <t>Total: 5k columns</t>
-  </si>
-  <si>
-    <t>DT1</t>
-  </si>
-  <si>
-    <t>DT2</t>
-  </si>
-  <si>
-    <t>DT3</t>
-  </si>
-  <si>
-    <t>DT4</t>
-  </si>
-  <si>
-    <t>DT5</t>
-  </si>
-  <si>
-    <t>DT6</t>
-  </si>
-  <si>
-    <t>Theo bảng date</t>
-  </si>
-  <si>
-    <t>I2004</t>
-  </si>
-  <si>
-    <t>I2005</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Theo bảng Demographic base on D_ID</t>
-  </si>
-  <si>
-    <t>Theo bảng Patient(base on P_ID)</t>
-  </si>
-  <si>
-    <t>Column6</t>
-  </si>
-  <si>
-    <t>Column7</t>
-  </si>
-  <si>
-    <t>Column8</t>
-  </si>
-  <si>
-    <t>Column9</t>
-  </si>
-  <si>
-    <t>Column10</t>
-  </si>
-  <si>
-    <t>Column11</t>
-  </si>
-  <si>
-    <t>Column12</t>
-  </si>
-  <si>
-    <t>Total: 5000 colums</t>
-  </si>
-  <si>
-    <t>Total: 32 columns</t>
-  </si>
-  <si>
-    <t>Total: 5 colums</t>
-  </si>
-  <si>
-    <t>Total: 1000 columns</t>
-  </si>
-  <si>
-    <t>Symptom_ID</t>
-  </si>
-  <si>
-    <t>Symptom_Name</t>
-  </si>
-  <si>
-    <t>Symptom_Stage</t>
-  </si>
-  <si>
-    <t>Symptom_Stage_Desc</t>
-  </si>
-  <si>
-    <t>Symptom_Repeated_Time</t>
-  </si>
-  <si>
-    <t>random(1,0)</t>
+    <t>Random(5000 times)</t>
   </si>
 </sst>
 </file>
@@ -834,13 +781,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -849,11 +792,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -879,59 +818,10 @@
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}" name="Table7" displayName="Table7" ref="A1:D13" totalsRowShown="0">
-  <autoFilter ref="A1:D13" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{82F6FD84-E924-495D-9C8C-D8D902D02007}" name="Column Name"/>
-    <tableColumn id="2" xr3:uid="{9EB30155-F8F4-4911-9394-0E8B659DAAA6}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{9D75EC3A-EE92-4C84-BF2B-9B7C70902EF5}" name="Key"/>
-    <tableColumn id="4" xr3:uid="{EB200C63-6CF0-430C-A0F9-513995D48DCB}" name="Note"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}" name="Table14" displayName="Table14" ref="F6:Q13" totalsRowShown="0">
-  <autoFilter ref="F6:Q13" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{7227021B-20F6-4823-AE83-785A5D6E3F88}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{64B431FB-56E7-42B2-A897-6C2F79451140}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{CF43519C-595E-44E5-8532-18F6EFF0E066}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{FABB793E-D151-4EA0-BE4C-09A512CB3310}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{EA02C3B5-5D63-4814-A336-83D143D9F5A2}" name="Column5"/>
-    <tableColumn id="6" xr3:uid="{74A8E224-A06E-4792-B2F6-F016675E9DB9}" name="Column6"/>
-    <tableColumn id="7" xr3:uid="{262255CF-99C4-4705-9430-CDA3734045CD}" name="Column7"/>
-    <tableColumn id="8" xr3:uid="{29CC84A4-0D3E-497D-9A21-7A19150143CA}" name="Column8"/>
-    <tableColumn id="9" xr3:uid="{63B02EB5-8B62-4692-91B0-6C39B73E5A76}" name="Column9"/>
-    <tableColumn id="10" xr3:uid="{569B60D3-E99F-4244-98FD-6901E280C441}" name="Column10"/>
-    <tableColumn id="11" xr3:uid="{1BC26F58-90ED-470B-8A35-E77C28D767B4}" name="Column11"/>
-    <tableColumn id="12" xr3:uid="{E301E0FD-788A-4E47-98FC-6BDFB2D5BF3D}" name="Column12"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{67587BFF-C6FA-4958-9F4F-61E542BE81AC}" name="Table3" displayName="Table3" ref="I4:N8" totalsRowShown="0">
-  <autoFilter ref="I4:N8" xr:uid="{67587BFF-C6FA-4958-9F4F-61E542BE81AC}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A9F3507B-86DC-472D-8FFF-E2C28B4B8B55}" name="Demographic_ID"/>
-    <tableColumn id="2" xr3:uid="{AD3F0BA4-5F91-4FB9-99D4-EFBA15DA14C3}" name="Patient_ID"/>
-    <tableColumn id="3" xr3:uid="{13337579-46BD-44D9-B7FC-95742E653730}" name="Insurance_ID"/>
-    <tableColumn id="4" xr3:uid="{30B8985B-9FFC-46CD-8E82-A39928CC2B42}" name="Insurance_Type"/>
-    <tableColumn id="5" xr3:uid="{6B737F95-637A-419E-A094-AC43553B7A57}" name="Insurance_Expired" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{17A7BEBD-FFCA-4AF3-9610-A7DAF4BE67EB}" name="History_Covid"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F74E800A-84A7-412D-A3FF-DF9CA2CACD42}" name="Table4" displayName="Table4" ref="I5:Q10" totalsRowShown="0">
-  <autoFilter ref="I5:Q10" xr:uid="{F74E800A-84A7-412D-A3FF-DF9CA2CACD42}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F74E800A-84A7-412D-A3FF-DF9CA2CACD42}" name="Table4" displayName="Table4" ref="I5:S10" totalsRowShown="0">
+  <autoFilter ref="I5:S10" xr:uid="{F74E800A-84A7-412D-A3FF-DF9CA2CACD42}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{707D9162-FC46-4776-B579-75668EEB95B6}" name="Patient_ID"/>
     <tableColumn id="2" xr3:uid="{75A00B8A-4C22-4F30-A0A9-8DA6F519568D}" name="Patient_Name"/>
     <tableColumn id="3" xr3:uid="{445A49D0-CEFE-4104-8743-5D55F064B2CD}" name="Patient_Gender"/>
@@ -941,12 +831,14 @@
     <tableColumn id="7" xr3:uid="{AC3F7D6F-4609-44F1-B7C1-30A9FD6996CA}" name="Patient_State"/>
     <tableColumn id="8" xr3:uid="{28CA7D2D-C2CB-4291-BA00-610F9B7BE7F0}" name="Patient_Bloodtype"/>
     <tableColumn id="9" xr3:uid="{1667010F-25BD-4200-8626-FA62547F6DB8}" name="Patient_Weight_kg"/>
+    <tableColumn id="10" xr3:uid="{76C7C799-EA04-4BF0-8E1B-F9AA6D006DE1}" name="History_Covid"/>
+    <tableColumn id="11" xr3:uid="{5DBAF08A-2133-4449-B1F8-0B5866FDF50E}" name="Insurance_ID"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1BF5BAA7-47F9-4C06-8533-2B4A8BB67E63}" name="Table1" displayName="Table1" ref="I6:L11" totalsRowShown="0">
   <autoFilter ref="I6:L11" xr:uid="{1BF5BAA7-47F9-4C06-8533-2B4A8BB67E63}"/>
   <tableColumns count="4">
@@ -959,7 +851,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E4C8AEE8-4517-4AA2-AA6B-380234F3FDBF}" name="Table2" displayName="Table2" ref="I6:M38" totalsRowShown="0">
   <autoFilter ref="I6:M38" xr:uid="{E4C8AEE8-4517-4AA2-AA6B-380234F3FDBF}"/>
   <tableColumns count="5">
@@ -973,7 +865,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{1911CEF0-3178-444A-AB4C-1FF818936319}" name="Table11" displayName="Table11" ref="A1:D7" totalsRowShown="0">
   <autoFilter ref="A1:D7" xr:uid="{1911CEF0-3178-444A-AB4C-1FF818936319}"/>
   <tableColumns count="4">
@@ -986,7 +878,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3D39A906-9290-4620-88D9-3D0E74A0723B}" name="Table6" displayName="Table6" ref="I5:L13" totalsRowShown="0">
   <autoFilter ref="I5:L13" xr:uid="{3D39A906-9290-4620-88D9-3D0E74A0723B}"/>
   <tableColumns count="4">
@@ -999,9 +891,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{02A19413-FB07-4759-A25F-021BF1EB9D67}" name="Table9" displayName="Table9" ref="A1:D5" totalsRowShown="0">
-  <autoFilter ref="A1:D5" xr:uid="{02A19413-FB07-4759-A25F-021BF1EB9D67}"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{02A19413-FB07-4759-A25F-021BF1EB9D67}" name="Table9" displayName="Table9" ref="A1:D6" totalsRowShown="0">
+  <autoFilter ref="A1:D6" xr:uid="{02A19413-FB07-4759-A25F-021BF1EB9D67}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C62703B6-F26D-4EE6-A104-1EA4B7BFB8C2}" name="Column Name"/>
     <tableColumn id="2" xr3:uid="{E783E5B4-4EFB-4973-B0C1-57515A5A1856}" name="Type"/>
@@ -1012,14 +904,31 @@
 </table>
 </file>
 
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}" name="Table7" displayName="Table7" ref="A1:D9" totalsRowShown="0">
+  <autoFilter ref="A1:D9" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{82F6FD84-E924-495D-9C8C-D8D902D02007}" name="Column Name"/>
+    <tableColumn id="2" xr3:uid="{9EB30155-F8F4-4911-9394-0E8B659DAAA6}" name="Type"/>
+    <tableColumn id="3" xr3:uid="{9D75EC3A-EE92-4C84-BF2B-9B7C70902EF5}" name="Key"/>
+    <tableColumn id="4" xr3:uid="{EB200C63-6CF0-430C-A0F9-513995D48DCB}" name="Note"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{97D9880E-DC69-4A7F-850A-56AF12EADD0C}" name="Table8" displayName="Table8" ref="A1:D4" totalsRowShown="0">
-  <autoFilter ref="A1:D4" xr:uid="{97D9880E-DC69-4A7F-850A-56AF12EADD0C}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{01A89381-BDEA-437D-9DFE-C61473529639}" name="Column Name"/>
-    <tableColumn id="2" xr3:uid="{2DFA2115-EA67-4D16-920A-251A87D12DF9}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{0AFE9AF5-8D46-47E0-B6B1-9D3A28508837}" name="Key"/>
-    <tableColumn id="4" xr3:uid="{35D0329C-1960-46F8-A84C-80253EEEEE6C}" name="Note"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}" name="Table14" displayName="Table14" ref="F6:M13" totalsRowShown="0">
+  <autoFilter ref="F6:M13" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{7227021B-20F6-4823-AE83-785A5D6E3F88}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{64B431FB-56E7-42B2-A897-6C2F79451140}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{CF43519C-595E-44E5-8532-18F6EFF0E066}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{FABB793E-D151-4EA0-BE4C-09A512CB3310}" name="Column4"/>
+    <tableColumn id="9" xr3:uid="{63B02EB5-8B62-4692-91B0-6C39B73E5A76}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{569B60D3-E99F-4244-98FD-6901E280C441}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{1BC26F58-90ED-470B-8A35-E77C28D767B4}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{E301E0FD-788A-4E47-98FC-6BDFB2D5BF3D}" name="Column12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1325,7 +1234,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,138 +1252,138 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>160</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E3" t="s">
         <v>174</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E3" t="s">
-        <v>183</v>
-      </c>
       <c r="I3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J3" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="K3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="L3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" t="s">
+        <v>169</v>
+      </c>
+      <c r="I4" t="s">
         <v>161</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" t="s">
-        <v>177</v>
-      </c>
-      <c r="I4" t="s">
-        <v>168</v>
       </c>
       <c r="J4">
         <v>6000</v>
       </c>
       <c r="K4" t="s">
-        <v>172</v>
-      </c>
-      <c r="L4" s="4">
+        <v>165</v>
+      </c>
+      <c r="L4" s="2">
         <v>45661</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>170</v>
+      </c>
+      <c r="I5" t="s">
         <v>162</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>178</v>
-      </c>
-      <c r="I5" t="s">
-        <v>169</v>
       </c>
       <c r="J5">
         <v>9000</v>
       </c>
       <c r="K5" t="s">
-        <v>179</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>181</v>
+        <v>171</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I6" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="J6">
         <v>6000</v>
       </c>
       <c r="K6" t="s">
-        <v>172</v>
-      </c>
-      <c r="L6" s="4">
+        <v>165</v>
+      </c>
+      <c r="L6" s="2">
         <v>45661</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J7">
         <v>9000</v>
       </c>
       <c r="K7" t="s">
-        <v>179</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>182</v>
+        <v>171</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>235</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -1487,226 +1396,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3AF490-97C9-4C79-9530-1AB0E3A32EE6}">
-  <dimension ref="A1:N12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7AF1BA3-C17A-4D61-9274-54FCDF565A10}">
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1"/>
-    <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>160</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>167</v>
-      </c>
-      <c r="I4" t="s">
-        <v>159</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>160</v>
-      </c>
-      <c r="L4" t="s">
-        <v>161</v>
-      </c>
-      <c r="M4" t="s">
-        <v>162</v>
-      </c>
-      <c r="N4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>164</v>
-      </c>
-      <c r="I5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" t="s">
-        <v>138</v>
-      </c>
-      <c r="K5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L5" t="s">
-        <v>172</v>
-      </c>
-      <c r="M5" s="2">
-        <v>45661</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>162</v>
-      </c>
-      <c r="B6" t="s">
-        <v>165</v>
-      </c>
-      <c r="D6" t="s">
-        <v>180</v>
-      </c>
-      <c r="I6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" t="s">
-        <v>139</v>
-      </c>
-      <c r="K6" t="s">
-        <v>169</v>
-      </c>
-      <c r="L6" t="s">
-        <v>173</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>241</v>
-      </c>
-      <c r="I7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" t="s">
-        <v>140</v>
-      </c>
-      <c r="K7" t="s">
-        <v>170</v>
-      </c>
-      <c r="L7" t="s">
-        <v>172</v>
-      </c>
-      <c r="M7" s="2">
-        <v>45661</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" t="s">
-        <v>141</v>
-      </c>
-      <c r="K8" t="s">
-        <v>171</v>
-      </c>
-      <c r="L8" t="s">
-        <v>173</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>235</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7AF1BA3-C17A-4D61-9274-54FCDF565A10}">
-  <dimension ref="A1:Q15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,289 +1416,349 @@
     <col min="15" max="15" width="15.140625" customWidth="1"/>
     <col min="16" max="16" width="19.7109375" customWidth="1"/>
     <col min="17" max="17" width="20.140625" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="I5" t="s">
         <v>1</v>
       </c>
       <c r="J5" t="s">
+        <v>122</v>
+      </c>
+      <c r="K5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" t="s">
+        <v>124</v>
+      </c>
+      <c r="N5" t="s">
         <v>125</v>
       </c>
-      <c r="K5" t="s">
+      <c r="O5" t="s">
         <v>126</v>
       </c>
-      <c r="L5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="P5" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>133</v>
+      </c>
+      <c r="R5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
         <v>127</v>
       </c>
-      <c r="N5" t="s">
-        <v>128</v>
-      </c>
-      <c r="O5" t="s">
-        <v>129</v>
-      </c>
-      <c r="P5" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>130</v>
-      </c>
       <c r="I6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="J6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="K6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="L6">
         <v>23</v>
       </c>
       <c r="M6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="N6">
         <v>60601</v>
       </c>
       <c r="O6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="P6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="Q6">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K7" t="s">
         <v>144</v>
-      </c>
-      <c r="K7" t="s">
-        <v>147</v>
       </c>
       <c r="L7">
         <v>24</v>
       </c>
       <c r="M7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="N7">
         <v>60601</v>
       </c>
       <c r="O7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="P7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q7">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="I8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="K8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="L8">
         <v>40</v>
       </c>
       <c r="M8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="N8">
         <v>60601</v>
       </c>
       <c r="O8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="P8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="Q8">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="L9">
         <v>79</v>
       </c>
       <c r="M9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="N9">
         <v>60601</v>
       </c>
       <c r="O9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="P9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q9">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="L10">
         <v>80</v>
       </c>
       <c r="M10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="N10">
         <v>60601</v>
       </c>
       <c r="O10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="P10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="Q10">
         <v>70</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>235</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -2016,12 +1770,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8961B12-14C4-41F4-847F-48839C9A3E3E}">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,144 +1794,144 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>234</v>
+        <v>212</v>
       </c>
       <c r="I9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" t="s">
         <v>34</v>
-      </c>
-      <c r="K11" t="s">
-        <v>38</v>
-      </c>
-      <c r="L11" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2189,12 +1943,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9772A3FD-BEF1-40F4-9572-5D20CC2045A5}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2211,642 +1965,642 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
         <v>40</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>237</v>
+        <v>215</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>238</v>
+        <v>216</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>236</v>
+        <v>214</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L7">
         <v>1</v>
       </c>
       <c r="M7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="M8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="I9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L9">
         <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L10">
         <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>233</v>
+        <v>211</v>
       </c>
       <c r="I11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L11">
         <v>1</v>
       </c>
       <c r="M11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L12">
         <v>2</v>
       </c>
       <c r="M12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L13">
         <v>2</v>
       </c>
       <c r="M13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L14">
         <v>2</v>
       </c>
       <c r="M14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L15">
         <v>1</v>
       </c>
       <c r="M15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L16">
         <v>1</v>
       </c>
       <c r="M16" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L17">
         <v>1</v>
       </c>
       <c r="M17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L18">
         <v>2</v>
       </c>
       <c r="M18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L19">
         <v>3</v>
       </c>
       <c r="M19" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I20" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J20" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K20" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L20">
         <v>1</v>
       </c>
       <c r="M20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J21" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K21" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L21">
         <v>1</v>
       </c>
       <c r="M21" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L22">
         <v>1</v>
       </c>
       <c r="M22" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="L23">
         <v>2</v>
       </c>
       <c r="M23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L24">
         <v>3</v>
       </c>
       <c r="M24" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I25" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K25" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="L25">
         <v>3</v>
       </c>
       <c r="M25" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K26" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L26">
         <v>3</v>
       </c>
       <c r="M26" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I27" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J27" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L27">
         <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K28" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L28">
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I29" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J29" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K29" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L29">
         <v>1</v>
       </c>
       <c r="M29" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I30" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J30" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K30" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="L30">
         <v>1</v>
       </c>
       <c r="M30" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I31" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J31" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L31">
         <v>2</v>
       </c>
       <c r="M31" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I32" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K32" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L32">
         <v>2</v>
       </c>
       <c r="M32" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I33" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J33" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K33" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L33">
         <v>1</v>
       </c>
       <c r="M33" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I34" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="J34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K34" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="L34">
         <v>2</v>
       </c>
       <c r="M34" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J35" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K35" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="L35">
         <v>3</v>
       </c>
       <c r="M35" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I36" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J36" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K36" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L36">
         <v>3</v>
       </c>
       <c r="M36" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I37" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J37" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K37" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L37">
         <v>3</v>
       </c>
       <c r="M37" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I38" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J38" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K38" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L38">
         <v>3</v>
       </c>
       <c r="M38" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2859,12 +2613,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6223762B-2B63-423A-B0E8-AA47018227CA}">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2879,16 +2633,16 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2896,69 +2650,81 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>236</v>
+        <v>214</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I5" t="s">
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>236</v>
+        <v>214</v>
       </c>
       <c r="K5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>224</v>
+      </c>
       <c r="I6" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="J6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -2969,10 +2735,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I7" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="J7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K7">
         <v>4</v>
@@ -2983,10 +2749,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I8" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="J8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K8">
         <v>5</v>
@@ -2997,13 +2763,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>232</v>
+        <v>210</v>
       </c>
       <c r="I9" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="J9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -3014,10 +2780,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="J10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -3028,10 +2794,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I11" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="J11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -3042,10 +2808,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I12" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -3056,10 +2822,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="J13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -3078,89 +2844,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28921E2C-DB16-4258-B853-A89027B508BE}">
-  <dimension ref="A1:D7"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DB1A5A-DDCB-4891-AFE3-44BA495796A4}">
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DB1A5A-DDCB-4891-AFE3-44BA495796A4}">
-  <dimension ref="A1:Q15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="F21" sqref="F21:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3175,140 +2864,125 @@
     <col min="9" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
     <col min="16" max="16" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" t="s">
         <v>40</v>
       </c>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" t="s">
-        <v>43</v>
-      </c>
       <c r="J6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="K6" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="L6" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="M6" t="s">
-        <v>227</v>
-      </c>
-      <c r="N6" t="s">
-        <v>228</v>
-      </c>
-      <c r="O6" t="s">
-        <v>229</v>
-      </c>
-      <c r="P6" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F7" t="s">
         <v>0</v>
@@ -3323,213 +2997,123 @@
         <v>3</v>
       </c>
       <c r="J7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M7" t="s">
-        <v>7</v>
-      </c>
-      <c r="N7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="O7" t="s">
-        <v>9</v>
-      </c>
-      <c r="P7" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
       <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>205</v>
+      </c>
+      <c r="F8" t="s">
+        <v>190</v>
+      </c>
+      <c r="G8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H8" t="s">
+        <v>178</v>
+      </c>
+      <c r="I8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
-        <v>203</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
         <v>205</v>
       </c>
-      <c r="G8" t="s">
-        <v>138</v>
-      </c>
-      <c r="H8" t="s">
-        <v>188</v>
-      </c>
-      <c r="I8" t="s">
-        <v>212</v>
-      </c>
-      <c r="J8" t="s">
-        <v>218</v>
-      </c>
-      <c r="K8" t="s">
-        <v>218</v>
-      </c>
-      <c r="L8" t="s">
-        <v>168</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>223</v>
-      </c>
       <c r="F9" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="G9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H9" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="I9" t="s">
-        <v>213</v>
-      </c>
-      <c r="L9" t="s">
-        <v>169</v>
-      </c>
-      <c r="M9" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>224</v>
-      </c>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="G10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H10" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="I10" t="s">
-        <v>214</v>
-      </c>
-      <c r="L10" t="s">
-        <v>170</v>
-      </c>
-      <c r="M10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>224</v>
-      </c>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="G11" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H11" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="I11" t="s">
-        <v>215</v>
-      </c>
-      <c r="L11" t="s">
-        <v>171</v>
-      </c>
-      <c r="M11" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>224</v>
-      </c>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="G12" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="I12" t="s">
-        <v>216</v>
-      </c>
-      <c r="L12" t="s">
-        <v>219</v>
-      </c>
-      <c r="M12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>224</v>
-      </c>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="G13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H13" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="I13" t="s">
-        <v>217</v>
-      </c>
-      <c r="L13" t="s">
-        <v>220</v>
-      </c>
-      <c r="M13" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Desc file and Model as requested.
- Change Insurance_Expired from Insurance table to random (year =2024)
- Change Appointment_Date from Diagnosis table to random(year =2021,2022)
- Delete Address from Patient table
-Put all the IDs on the top from each Tables
- Add Appointment_Date from Diagnosis table
- Delete Date_ID From Medical and Insurance_Number
- Add History_Covid and Appointment_Date for Medical Table
- Add Blood_Pressure_mmHg and Blood_Sugar_mgDl to Patient table
</commit_message>
<xml_diff>
--- a/docs/Desc and Example Tables.xlsx
+++ b/docs/Desc and Example Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17737\Desktop\FPT\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926A63C4-662C-4881-832A-4BF20C39C4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB3A68E-0CC0-4CB1-BF20-A3E2293B96BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="15" windowWidth="28800" windowHeight="16185" activeTab="3" xr2:uid="{76F2D5F5-96DF-42B7-9620-589D1FA50423}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{76F2D5F5-96DF-42B7-9620-589D1FA50423}"/>
   </bookViews>
   <sheets>
     <sheet name="Insurance" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="212">
   <si>
     <t>Medical_ID</t>
   </si>
@@ -50,12 +50,6 @@
     <t>Diagnosis_ID</t>
   </si>
   <si>
-    <t>Date_ID</t>
-  </si>
-  <si>
-    <t>Insurance_Number</t>
-  </si>
-  <si>
     <t>History_Covid</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
     <t>Patient_Age</t>
   </si>
   <si>
-    <t>Bloor_Pressure_mmHg</t>
-  </si>
-  <si>
     <t>Column Name</t>
   </si>
   <si>
@@ -413,9 +404,6 @@
     <t>Patient_Gender</t>
   </si>
   <si>
-    <t>Patient_Address</t>
-  </si>
-  <si>
     <t>Patient_Zip</t>
   </si>
   <si>
@@ -479,21 +467,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>123 Washington St</t>
-  </si>
-  <si>
-    <t>124 Washington St</t>
-  </si>
-  <si>
-    <t>125 Washington St</t>
-  </si>
-  <si>
-    <t>126 Washington St</t>
-  </si>
-  <si>
-    <t>127 Washington St</t>
-  </si>
-  <si>
     <t>IL</t>
   </si>
   <si>
@@ -551,15 +524,9 @@
     <t>random (HMO. PPO)</t>
   </si>
   <si>
-    <t>giống với bảng Demographic</t>
-  </si>
-  <si>
     <t>PMO</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1/4/2023</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 10/5/2024</t>
   </si>
   <si>
@@ -608,9 +575,6 @@
     <t>random P1-P1000 (5000 lần)</t>
   </si>
   <si>
-    <t>random (I2000-I3000)</t>
-  </si>
-  <si>
     <t>M1</t>
   </si>
   <si>
@@ -629,27 +593,6 @@
     <t>M6</t>
   </si>
   <si>
-    <t>Total: 5k columns</t>
-  </si>
-  <si>
-    <t>DT1</t>
-  </si>
-  <si>
-    <t>DT2</t>
-  </si>
-  <si>
-    <t>DT3</t>
-  </si>
-  <si>
-    <t>DT4</t>
-  </si>
-  <si>
-    <t>DT5</t>
-  </si>
-  <si>
-    <t>DT6</t>
-  </si>
-  <si>
     <t>I2004</t>
   </si>
   <si>
@@ -659,18 +602,6 @@
     <t>Theo bảng Patient(base on P_ID)</t>
   </si>
   <si>
-    <t>Column9</t>
-  </si>
-  <si>
-    <t>Column10</t>
-  </si>
-  <si>
-    <t>Column11</t>
-  </si>
-  <si>
-    <t>Column12</t>
-  </si>
-  <si>
     <t>Total: 5000 colums</t>
   </si>
   <si>
@@ -698,9 +629,6 @@
     <t>Symptom_Repeated_Time</t>
   </si>
   <si>
-    <t>random(1, 0)</t>
-  </si>
-  <si>
     <t>Random (I2000-I3000)</t>
   </si>
   <si>
@@ -713,7 +641,40 @@
     <t>date</t>
   </si>
   <si>
-    <t>Random(5000 times)</t>
+    <t>random (year = 2024)</t>
+  </si>
+  <si>
+    <t>Random(5000 times) (Year = 2021,2022)</t>
+  </si>
+  <si>
+    <t>a-b-2021</t>
+  </si>
+  <si>
+    <t>a-b-2022</t>
+  </si>
+  <si>
+    <t>Total: 5000 columns</t>
+  </si>
+  <si>
+    <t>Random range(120-200)</t>
+  </si>
+  <si>
+    <t>Random(1, 0)</t>
+  </si>
+  <si>
+    <t>Random range(100- 200)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1/4/2024</t>
+  </si>
+  <si>
+    <t>Blood_Pressure_mmHG</t>
+  </si>
+  <si>
+    <t>Blodd_Sugar_mgdL</t>
+  </si>
+  <si>
+    <t>Theo bảng Diagnosis(base on Dianosis_ID)</t>
   </si>
 </sst>
 </file>
@@ -819,20 +780,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F74E800A-84A7-412D-A3FF-DF9CA2CACD42}" name="Table4" displayName="Table4" ref="I5:S10" totalsRowShown="0">
-  <autoFilter ref="I5:S10" xr:uid="{F74E800A-84A7-412D-A3FF-DF9CA2CACD42}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F74E800A-84A7-412D-A3FF-DF9CA2CACD42}" name="Table4" displayName="Table4" ref="I6:T11" totalsRowShown="0">
+  <autoFilter ref="I6:T11" xr:uid="{F74E800A-84A7-412D-A3FF-DF9CA2CACD42}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{707D9162-FC46-4776-B579-75668EEB95B6}" name="Patient_ID"/>
+    <tableColumn id="11" xr3:uid="{5DBAF08A-2133-4449-B1F8-0B5866FDF50E}" name="Insurance_ID"/>
     <tableColumn id="2" xr3:uid="{75A00B8A-4C22-4F30-A0A9-8DA6F519568D}" name="Patient_Name"/>
     <tableColumn id="3" xr3:uid="{445A49D0-CEFE-4104-8743-5D55F064B2CD}" name="Patient_Gender"/>
     <tableColumn id="4" xr3:uid="{2FEB4D4B-F500-4A1B-8F84-7347C93A4F77}" name="Patient_Age"/>
-    <tableColumn id="5" xr3:uid="{1F32C101-C3CB-4D86-AEBB-75607A94CE5D}" name="Patient_Address"/>
     <tableColumn id="6" xr3:uid="{A82F1155-0E7C-4787-A01C-210D48BB285D}" name="Patient_Zip"/>
     <tableColumn id="7" xr3:uid="{AC3F7D6F-4609-44F1-B7C1-30A9FD6996CA}" name="Patient_State"/>
     <tableColumn id="8" xr3:uid="{28CA7D2D-C2CB-4291-BA00-610F9B7BE7F0}" name="Patient_Bloodtype"/>
     <tableColumn id="9" xr3:uid="{1667010F-25BD-4200-8626-FA62547F6DB8}" name="Patient_Weight_kg"/>
     <tableColumn id="10" xr3:uid="{76C7C799-EA04-4BF0-8E1B-F9AA6D006DE1}" name="History_Covid"/>
-    <tableColumn id="11" xr3:uid="{5DBAF08A-2133-4449-B1F8-0B5866FDF50E}" name="Insurance_ID"/>
+    <tableColumn id="5" xr3:uid="{4B915945-77F1-40AB-BEEA-B907A7B3C597}" name="Blood_Pressure_mmHG"/>
+    <tableColumn id="12" xr3:uid="{BC631972-A28E-4C76-9BA3-008881FFD9C1}" name="Blodd_Sugar_mgdL"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -879,11 +841,12 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3D39A906-9290-4620-88D9-3D0E74A0723B}" name="Table6" displayName="Table6" ref="I5:L13" totalsRowShown="0">
-  <autoFilter ref="I5:L13" xr:uid="{3D39A906-9290-4620-88D9-3D0E74A0723B}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3D39A906-9290-4620-88D9-3D0E74A0723B}" name="Table6" displayName="Table6" ref="I5:M13" totalsRowShown="0">
+  <autoFilter ref="I5:M13" xr:uid="{3D39A906-9290-4620-88D9-3D0E74A0723B}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8B92FE1E-E55E-4D2C-9DD5-FF786D76CF38}" name="Diagnosis_ID"/>
     <tableColumn id="2" xr3:uid="{A00622D6-26D8-4327-8BDB-F4490C333D60}" name="Symptom_ID"/>
+    <tableColumn id="5" xr3:uid="{36988D2B-84DA-4DF0-9ABB-712017EB4C11}" name="Appointment_Date"/>
     <tableColumn id="3" xr3:uid="{C12F9D53-8CEA-446C-925B-45B03D048F80}" name="Symtom_Repeated_Time"/>
     <tableColumn id="4" xr3:uid="{E2BBC69F-57BF-44C4-B75E-BD7E94525595}" name="Probability_Diagnosis"/>
   </tableColumns>
@@ -905,8 +868,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}" name="Table7" displayName="Table7" ref="A1:D9" totalsRowShown="0">
-  <autoFilter ref="A1:D9" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}" name="Table7" displayName="Table7" ref="A1:D10" totalsRowShown="0">
+  <autoFilter ref="A1:D10" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{82F6FD84-E924-495D-9C8C-D8D902D02007}" name="Column Name"/>
     <tableColumn id="2" xr3:uid="{9EB30155-F8F4-4911-9394-0E8B659DAAA6}" name="Type"/>
@@ -918,17 +881,18 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}" name="Table14" displayName="Table14" ref="F6:M13" totalsRowShown="0">
-  <autoFilter ref="F6:M13" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{7227021B-20F6-4823-AE83-785A5D6E3F88}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{64B431FB-56E7-42B2-A897-6C2F79451140}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{CF43519C-595E-44E5-8532-18F6EFF0E066}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{FABB793E-D151-4EA0-BE4C-09A512CB3310}" name="Column4"/>
-    <tableColumn id="9" xr3:uid="{63B02EB5-8B62-4692-91B0-6C39B73E5A76}" name="Column9"/>
-    <tableColumn id="10" xr3:uid="{569B60D3-E99F-4244-98FD-6901E280C441}" name="Column10"/>
-    <tableColumn id="11" xr3:uid="{1BC26F58-90ED-470B-8A35-E77C28D767B4}" name="Column11"/>
-    <tableColumn id="12" xr3:uid="{E301E0FD-788A-4E47-98FC-6BDFB2D5BF3D}" name="Column12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}" name="Table14" displayName="Table14" ref="F7:N13" totalsRowShown="0">
+  <autoFilter ref="F7:N13" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{7227021B-20F6-4823-AE83-785A5D6E3F88}" name="Medical_ID"/>
+    <tableColumn id="2" xr3:uid="{64B431FB-56E7-42B2-A897-6C2F79451140}" name="Patient_ID"/>
+    <tableColumn id="3" xr3:uid="{CF43519C-595E-44E5-8532-18F6EFF0E066}" name="Diagnosis_ID"/>
+    <tableColumn id="4" xr3:uid="{FABB793E-D151-4EA0-BE4C-09A512CB3310}" name="Appointment_Date"/>
+    <tableColumn id="9" xr3:uid="{63B02EB5-8B62-4692-91B0-6C39B73E5A76}" name="Patient_Weight"/>
+    <tableColumn id="10" xr3:uid="{569B60D3-E99F-4244-98FD-6901E280C441}" name="Patient_Age"/>
+    <tableColumn id="11" xr3:uid="{1BC26F58-90ED-470B-8A35-E77C28D767B4}" name="Blood_Pressure_mmHg"/>
+    <tableColumn id="12" xr3:uid="{E301E0FD-788A-4E47-98FC-6BDFB2D5BF3D}" name="Blood_Sugar_mgdL"/>
+    <tableColumn id="5" xr3:uid="{9E642A0A-BCCF-41DE-937D-8C8BE45F3AAC}" name="History_Covid"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1234,7 +1198,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,138 +1216,138 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="E3" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="I3" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="J3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="K3" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="L3" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D4" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I4" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="J4">
         <v>6000</v>
       </c>
       <c r="K4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="L4" s="2">
-        <v>45661</v>
+        <v>45295</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="I5" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="J5">
         <v>9000</v>
       </c>
       <c r="K5" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>172</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I6" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="J6">
         <v>6000</v>
       </c>
       <c r="K6" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="L6" s="2">
-        <v>45661</v>
+        <v>45295</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I7" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="J7">
         <v>9000</v>
       </c>
       <c r="K7" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -1397,368 +1361,401 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7AF1BA3-C17A-4D61-9274-54FCDF565A10}">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" customWidth="1"/>
     <col min="10" max="10" width="15.85546875" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" customWidth="1"/>
-    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.7109375" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" customWidth="1"/>
     <col min="15" max="15" width="15.140625" customWidth="1"/>
     <col min="16" max="16" width="19.7109375" customWidth="1"/>
     <col min="17" max="17" width="20.140625" customWidth="1"/>
     <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
       <c r="D2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>147</v>
+      </c>
+      <c r="K6" t="s">
+        <v>119</v>
+      </c>
+      <c r="L6" t="s">
+        <v>120</v>
+      </c>
+      <c r="M6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N6" t="s">
+        <v>121</v>
+      </c>
+      <c r="O6" t="s">
         <v>122</v>
       </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="P6" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="Q6" t="s">
         <v>129</v>
       </c>
-      <c r="I5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>122</v>
-      </c>
-      <c r="K5" t="s">
-        <v>123</v>
-      </c>
-      <c r="L5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" t="s">
-        <v>124</v>
-      </c>
-      <c r="N5" t="s">
-        <v>125</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="R6" t="s">
+        <v>3</v>
+      </c>
+      <c r="S6" t="s">
+        <v>209</v>
+      </c>
+      <c r="T6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
         <v>126</v>
       </c>
-      <c r="P5" t="s">
+      <c r="I7" t="s">
         <v>131</v>
       </c>
-      <c r="Q5" t="s">
-        <v>133</v>
-      </c>
-      <c r="R5" t="s">
-        <v>5</v>
-      </c>
-      <c r="S5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>127</v>
-      </c>
-      <c r="I6" t="s">
-        <v>135</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="J7" t="s">
+        <v>153</v>
+      </c>
+      <c r="K7" t="s">
+        <v>136</v>
+      </c>
+      <c r="L7" t="s">
         <v>140</v>
       </c>
-      <c r="K6" t="s">
-        <v>144</v>
-      </c>
-      <c r="L6">
+      <c r="M7">
         <v>23</v>
-      </c>
-      <c r="M6" t="s">
-        <v>146</v>
-      </c>
-      <c r="N6">
-        <v>60601</v>
-      </c>
-      <c r="O6" t="s">
-        <v>151</v>
-      </c>
-      <c r="P6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q6">
-        <v>70</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>130</v>
-      </c>
-      <c r="I7" t="s">
-        <v>136</v>
-      </c>
-      <c r="J7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K7" t="s">
-        <v>144</v>
-      </c>
-      <c r="L7">
-        <v>24</v>
-      </c>
-      <c r="M7" t="s">
-        <v>147</v>
       </c>
       <c r="N7">
         <v>60601</v>
       </c>
       <c r="O7" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="P7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="Q7">
         <v>70</v>
       </c>
       <c r="R7">
-        <v>1</v>
-      </c>
-      <c r="S7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>120</v>
+      </c>
+      <c r="T7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J8" t="s">
+        <v>185</v>
+      </c>
+      <c r="K8" t="s">
         <v>137</v>
       </c>
-      <c r="J8" t="s">
-        <v>142</v>
-      </c>
-      <c r="K8" t="s">
-        <v>144</v>
-      </c>
-      <c r="L8">
-        <v>40</v>
-      </c>
-      <c r="M8" t="s">
-        <v>148</v>
+      <c r="L8" t="s">
+        <v>140</v>
+      </c>
+      <c r="M8">
+        <v>24</v>
       </c>
       <c r="N8">
         <v>60601</v>
       </c>
       <c r="O8" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="P8" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="Q8">
         <v>70</v>
       </c>
       <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>121</v>
+      </c>
+      <c r="T8">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I9" t="s">
+        <v>133</v>
+      </c>
+      <c r="J9" t="s">
+        <v>197</v>
+      </c>
+      <c r="K9" t="s">
         <v>138</v>
       </c>
-      <c r="J9" t="s">
-        <v>27</v>
-      </c>
-      <c r="K9" t="s">
-        <v>145</v>
-      </c>
-      <c r="L9">
-        <v>79</v>
-      </c>
-      <c r="M9" t="s">
-        <v>149</v>
+      <c r="L9" t="s">
+        <v>140</v>
+      </c>
+      <c r="M9">
+        <v>40</v>
       </c>
       <c r="N9">
         <v>60601</v>
       </c>
       <c r="O9" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="P9" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="Q9">
         <v>70</v>
       </c>
       <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="S9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>122</v>
+      </c>
+      <c r="T9">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
+        <v>130</v>
+      </c>
+      <c r="I10" t="s">
         <v>134</v>
       </c>
-      <c r="I10" t="s">
-        <v>139</v>
-      </c>
       <c r="J10" t="s">
-        <v>143</v>
+        <v>184</v>
       </c>
       <c r="K10" t="s">
-        <v>145</v>
-      </c>
-      <c r="L10">
-        <v>80</v>
-      </c>
-      <c r="M10" t="s">
-        <v>150</v>
+        <v>24</v>
+      </c>
+      <c r="L10" t="s">
+        <v>141</v>
+      </c>
+      <c r="M10">
+        <v>79</v>
       </c>
       <c r="N10">
         <v>60601</v>
       </c>
       <c r="O10" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="P10" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="Q10">
         <v>70</v>
       </c>
       <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>123</v>
+      </c>
+      <c r="T10">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>206</v>
+      </c>
+      <c r="I11" t="s">
+        <v>135</v>
+      </c>
+      <c r="J11" t="s">
+        <v>185</v>
+      </c>
+      <c r="K11" t="s">
+        <v>139</v>
+      </c>
+      <c r="L11" t="s">
+        <v>141</v>
+      </c>
+      <c r="M11">
+        <v>80</v>
+      </c>
+      <c r="N11">
+        <v>60601</v>
+      </c>
+      <c r="O11" t="s">
+        <v>144</v>
+      </c>
+      <c r="P11" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q11">
+        <v>70</v>
+      </c>
+      <c r="R11">
         <v>0</v>
       </c>
-      <c r="S10" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S11">
+        <v>124</v>
+      </c>
+      <c r="T11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>213</v>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -1794,144 +1791,144 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="I9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" t="s">
         <v>31</v>
-      </c>
-      <c r="K11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L11" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1947,8 +1944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9772A3FD-BEF1-40F4-9572-5D20CC2045A5}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1956,7 +1953,7 @@
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" customWidth="1"/>
     <col min="11" max="11" width="46.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.28515625" customWidth="1"/>
@@ -1965,642 +1962,642 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
         <v>37</v>
-      </c>
-      <c r="B1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I6" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L7">
         <v>1</v>
       </c>
       <c r="M7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="M8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="I9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L9">
         <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L10">
         <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="I11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L11">
         <v>1</v>
       </c>
       <c r="M11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L12">
         <v>2</v>
       </c>
       <c r="M12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L13">
         <v>2</v>
       </c>
       <c r="M13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L14">
         <v>2</v>
       </c>
       <c r="M14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L15">
         <v>1</v>
       </c>
       <c r="M15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L16">
         <v>1</v>
       </c>
       <c r="M16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L17">
         <v>1</v>
       </c>
       <c r="M17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L18">
         <v>2</v>
       </c>
       <c r="M18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L19">
         <v>3</v>
       </c>
       <c r="M19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L20">
         <v>1</v>
       </c>
       <c r="M20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L21">
         <v>1</v>
       </c>
       <c r="M21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L22">
         <v>1</v>
       </c>
       <c r="M22" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K23" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L23">
         <v>2</v>
       </c>
       <c r="M23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J24" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L24">
         <v>3</v>
       </c>
       <c r="M24" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J25" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L25">
         <v>3</v>
       </c>
       <c r="M25" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J26" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="L26">
         <v>3</v>
       </c>
       <c r="M26" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K27" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L27">
         <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J28" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L28">
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I29" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K29" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="L29">
         <v>1</v>
       </c>
       <c r="M29" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I30" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J30" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K30" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L30">
         <v>1</v>
       </c>
       <c r="M30" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I31" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J31" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K31" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L31">
         <v>2</v>
       </c>
       <c r="M31" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I32" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J32" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K32" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L32">
         <v>2</v>
       </c>
       <c r="M32" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I33" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J33" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K33" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L33">
         <v>1</v>
       </c>
       <c r="M33" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I34" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J34" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K34" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="L34">
         <v>2</v>
       </c>
       <c r="M34" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I35" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J35" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="L35">
         <v>3</v>
       </c>
       <c r="M35" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I36" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J36" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K36" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L36">
         <v>3</v>
       </c>
       <c r="M36" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I37" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="J37" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K37" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="L37">
         <v>3</v>
       </c>
       <c r="M37" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I38" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K38" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="L38">
         <v>3</v>
       </c>
       <c r="M38" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2615,222 +2612,250 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6223762B-2B63-423A-B0E8-AA47018227CA}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K6" sqref="K6:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.42578125" customWidth="1"/>
-    <col min="12" max="12" width="22.28515625" customWidth="1"/>
+    <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
       <c r="D2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>199</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>195</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I5" t="s">
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="K5" t="s">
-        <v>119</v>
+        <v>198</v>
       </c>
       <c r="L5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="M5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>222</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>223</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>224</v>
+        <v>118</v>
       </c>
       <c r="I6" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="J6" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6">
+        <v>45</v>
+      </c>
+      <c r="K6" t="s">
+        <v>202</v>
+      </c>
+      <c r="L6">
         <v>1</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I7" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="J7" t="s">
-        <v>104</v>
-      </c>
-      <c r="K7">
+        <v>101</v>
+      </c>
+      <c r="K7" t="s">
+        <v>203</v>
+      </c>
+      <c r="L7">
         <v>4</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I8" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="J8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" t="s">
+        <v>203</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>187</v>
+      </c>
+      <c r="I9" t="s">
+        <v>170</v>
+      </c>
+      <c r="J9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" t="s">
+        <v>202</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>171</v>
+      </c>
+      <c r="J10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" t="s">
+        <v>203</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>172</v>
+      </c>
+      <c r="J11" t="s">
         <v>57</v>
       </c>
-      <c r="K8">
-        <v>5</v>
-      </c>
-      <c r="L8">
+      <c r="K11" t="s">
+        <v>202</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>210</v>
-      </c>
-      <c r="I9" t="s">
-        <v>181</v>
-      </c>
-      <c r="J9" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>173</v>
+      </c>
+      <c r="J12" t="s">
         <v>58</v>
       </c>
-      <c r="K9">
+      <c r="K12" t="s">
+        <v>203</v>
+      </c>
+      <c r="L12">
         <v>1</v>
       </c>
-      <c r="L9">
+      <c r="M12">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I10" t="s">
-        <v>182</v>
-      </c>
-      <c r="J10" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>174</v>
+      </c>
+      <c r="J13" t="s">
         <v>59</v>
       </c>
-      <c r="K10">
+      <c r="K13" t="s">
+        <v>202</v>
+      </c>
+      <c r="L13">
         <v>1</v>
       </c>
-      <c r="L10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I11" t="s">
-        <v>183</v>
-      </c>
-      <c r="J11" t="s">
-        <v>60</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I12" t="s">
-        <v>184</v>
-      </c>
-      <c r="J12" t="s">
-        <v>61</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I13" t="s">
-        <v>185</v>
-      </c>
-      <c r="J13" t="s">
-        <v>62</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
+      <c r="M13">
         <v>10</v>
       </c>
     </row>
@@ -2846,10 +2871,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DB1A5A-DDCB-4891-AFE3-44BA495796A4}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2857,132 +2882,109 @@
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
     <col min="16" max="16" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
       <c r="D2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>205</v>
-      </c>
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" t="s">
-        <v>206</v>
-      </c>
-      <c r="K6" t="s">
-        <v>207</v>
-      </c>
-      <c r="L6" t="s">
-        <v>208</v>
-      </c>
-      <c r="M6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="F7" t="s">
         <v>0</v>
@@ -2994,126 +2996,213 @@
         <v>2</v>
       </c>
       <c r="I7" t="s">
+        <v>198</v>
+      </c>
+      <c r="J7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" t="s">
         <v>3</v>
       </c>
-      <c r="J7" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L7" t="s">
-        <v>8</v>
-      </c>
-      <c r="M7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="F8" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="G8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H8" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="I8" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="J8">
+        <v>70</v>
+      </c>
+      <c r="K8">
+        <v>24</v>
+      </c>
+      <c r="L8">
+        <v>100</v>
+      </c>
+      <c r="M8">
+        <v>100</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="F9" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="G9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H9" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="I9" t="s">
+        <v>203</v>
+      </c>
+      <c r="J9">
+        <v>70</v>
+      </c>
+      <c r="K9">
+        <v>25</v>
+      </c>
+      <c r="L9">
+        <v>130</v>
+      </c>
+      <c r="M9">
+        <v>129</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>186</v>
+      </c>
+      <c r="F10" t="s">
+        <v>180</v>
+      </c>
+      <c r="G10" t="s">
+        <v>132</v>
+      </c>
+      <c r="H10" t="s">
+        <v>169</v>
+      </c>
+      <c r="I10" t="s">
+        <v>203</v>
+      </c>
+      <c r="J10">
+        <v>70</v>
+      </c>
+      <c r="K10">
+        <v>36</v>
+      </c>
+      <c r="L10">
+        <v>140</v>
+      </c>
+      <c r="M10">
         <v>198</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
-        <v>192</v>
-      </c>
-      <c r="G10" t="s">
-        <v>136</v>
-      </c>
-      <c r="H10" t="s">
-        <v>180</v>
-      </c>
-      <c r="I10" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="G11" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H11" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="I11" t="s">
+        <v>202</v>
+      </c>
+      <c r="J11">
+        <v>70</v>
+      </c>
+      <c r="K11">
+        <v>27</v>
+      </c>
+      <c r="L11">
+        <v>146</v>
+      </c>
+      <c r="M11">
         <v>200</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="G12" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H12" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="I12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="J12">
+        <v>70</v>
+      </c>
+      <c r="K12">
+        <v>48</v>
+      </c>
+      <c r="L12">
+        <v>200</v>
+      </c>
+      <c r="M12">
+        <v>141</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="G13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H13" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="I13" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>196</v>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update new Desc file and Data Model
- Add new table Dim_Date with attributes: Date_ID, Appointment_Date, Day, Month, Year, Quarter, Day_Of_Week.
- Delete Appointment_Date from Diagnosis table.
- Add Date_ID and Appointment_Date to Medical table.
</commit_message>
<xml_diff>
--- a/docs/Desc and Example Tables.xlsx
+++ b/docs/Desc and Example Tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17737\Desktop\FPT\Project 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17737\Desktop\FPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64821B9E-7C63-4908-809A-4078D3333888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDE5887-9BA6-4987-9514-2107B8106FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="1350" windowWidth="28800" windowHeight="16185" activeTab="4" xr2:uid="{76F2D5F5-96DF-42B7-9620-589D1FA50423}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{76F2D5F5-96DF-42B7-9620-589D1FA50423}"/>
   </bookViews>
   <sheets>
     <sheet name="Insurance" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Disease" sheetId="5" r:id="rId3"/>
     <sheet name="Symptom" sheetId="6" r:id="rId4"/>
     <sheet name="Diagnosis" sheetId="7" r:id="rId5"/>
-    <sheet name="Medical" sheetId="1" r:id="rId6"/>
+    <sheet name="Date" sheetId="8" r:id="rId6"/>
+    <sheet name="Medical" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="226">
   <si>
     <t>Medical_ID</t>
   </si>
@@ -671,10 +672,52 @@
     <t>Blodd_Sugar_mgdL</t>
   </si>
   <si>
-    <t>Theo bảng Diagnosis(base on Dianosis_ID)</t>
-  </si>
-  <si>
     <t>Random(5000 times) (Year between 2019 -2021)</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Date_ID</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Quarter</t>
+  </si>
+  <si>
+    <t>Day_Of_Week</t>
+  </si>
+  <si>
+    <t>DT(1-5000)</t>
+  </si>
+  <si>
+    <t>Day base on Appoiment_Date</t>
+  </si>
+  <si>
+    <t>Month base on Appoiment_Date</t>
+  </si>
+  <si>
+    <t>Year base on Appoiment_Date</t>
+  </si>
+  <si>
+    <t>Base on Month(1-&gt;3 = 3 -&gt; 6 =2,.. 9 -&gt; 12 = 4)</t>
+  </si>
+  <si>
+    <t>use format Month-Day-Year</t>
+  </si>
+  <si>
+    <t>Random DT(1-5000)</t>
+  </si>
+  <si>
+    <t>Theo bảng Date(base on Date_ID)</t>
   </si>
 </sst>
 </file>
@@ -742,18 +785,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -774,6 +828,25 @@
     <tableColumn id="2" xr3:uid="{43A7CF1E-6DA7-42A6-BB3C-7375AFBFC8EC}" name="Insurance_Cover_Ammount"/>
     <tableColumn id="3" xr3:uid="{35421352-61FA-438F-8AF4-BCEFA7F89966}" name="Insurance_Type"/>
     <tableColumn id="4" xr3:uid="{57F3944B-545F-44A1-BAED-610981CC9597}" name="Insurance_Expired"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}" name="Table14" displayName="Table14" ref="F8:O14" totalsRowShown="0">
+  <autoFilter ref="F8:O14" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{7227021B-20F6-4823-AE83-785A5D6E3F88}" name="Medical_ID"/>
+    <tableColumn id="2" xr3:uid="{64B431FB-56E7-42B2-A897-6C2F79451140}" name="Patient_ID"/>
+    <tableColumn id="3" xr3:uid="{CF43519C-595E-44E5-8532-18F6EFF0E066}" name="Diagnosis_ID"/>
+    <tableColumn id="7" xr3:uid="{E8BE27C5-42CD-4730-BA30-99000F8955AF}" name="Date_ID"/>
+    <tableColumn id="4" xr3:uid="{FABB793E-D151-4EA0-BE4C-09A512CB3310}" name="Appointment_Date" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{63B02EB5-8B62-4692-91B0-6C39B73E5A76}" name="Patient_Weight"/>
+    <tableColumn id="10" xr3:uid="{569B60D3-E99F-4244-98FD-6901E280C441}" name="Patient_Age"/>
+    <tableColumn id="11" xr3:uid="{1BC26F58-90ED-470B-8A35-E77C28D767B4}" name="Blood_Pressure_mmHg"/>
+    <tableColumn id="12" xr3:uid="{E301E0FD-788A-4E47-98FC-6BDFB2D5BF3D}" name="Blood_Sugar_mgdL"/>
+    <tableColumn id="5" xr3:uid="{9E642A0A-BCCF-41DE-937D-8C8BE45F3AAC}" name="History_Covid"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -868,31 +941,29 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}" name="Table7" displayName="Table7" ref="A1:D10" totalsRowShown="0">
-  <autoFilter ref="A1:D10" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{82F6FD84-E924-495D-9C8C-D8D902D02007}" name="Column Name"/>
-    <tableColumn id="2" xr3:uid="{9EB30155-F8F4-4911-9394-0E8B659DAAA6}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{9D75EC3A-EE92-4C84-BF2B-9B7C70902EF5}" name="Key"/>
-    <tableColumn id="4" xr3:uid="{EB200C63-6CF0-430C-A0F9-513995D48DCB}" name="Note"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8D386086-412F-4F15-B57A-3524CD3A74AA}" name="Table3" displayName="Table3" ref="I4:O9" totalsRowShown="0">
+  <autoFilter ref="I4:O9" xr:uid="{8D386086-412F-4F15-B57A-3524CD3A74AA}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{A202697D-1FEA-4478-A5FB-08AD456971F0}" name="Date_ID"/>
+    <tableColumn id="2" xr3:uid="{D24A4C43-A5DC-409B-BAB6-D3A7D35C28F3}" name="Appointment_Date" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{B9B3969D-11B2-401B-B112-79537FC98542}" name="Day"/>
+    <tableColumn id="4" xr3:uid="{E91D160C-CEF2-468E-B92F-85F7541A1661}" name="Month"/>
+    <tableColumn id="5" xr3:uid="{1862BDC0-7D95-41DE-A1A2-B187644035A7}" name="Year"/>
+    <tableColumn id="6" xr3:uid="{4F990E3D-CB8C-4D22-AB85-94E8893F531B}" name="Quarter"/>
+    <tableColumn id="7" xr3:uid="{CDEA9271-8A42-4757-9C7A-0F971EA26F77}" name="Day_Of_Week"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}" name="Table14" displayName="Table14" ref="F7:N13" totalsRowShown="0">
-  <autoFilter ref="F7:N13" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{7227021B-20F6-4823-AE83-785A5D6E3F88}" name="Medical_ID"/>
-    <tableColumn id="2" xr3:uid="{64B431FB-56E7-42B2-A897-6C2F79451140}" name="Patient_ID"/>
-    <tableColumn id="3" xr3:uid="{CF43519C-595E-44E5-8532-18F6EFF0E066}" name="Diagnosis_ID"/>
-    <tableColumn id="4" xr3:uid="{FABB793E-D151-4EA0-BE4C-09A512CB3310}" name="Appointment_Date"/>
-    <tableColumn id="9" xr3:uid="{63B02EB5-8B62-4692-91B0-6C39B73E5A76}" name="Patient_Weight"/>
-    <tableColumn id="10" xr3:uid="{569B60D3-E99F-4244-98FD-6901E280C441}" name="Patient_Age"/>
-    <tableColumn id="11" xr3:uid="{1BC26F58-90ED-470B-8A35-E77C28D767B4}" name="Blood_Pressure_mmHg"/>
-    <tableColumn id="12" xr3:uid="{E301E0FD-788A-4E47-98FC-6BDFB2D5BF3D}" name="Blood_Sugar_mgdL"/>
-    <tableColumn id="5" xr3:uid="{9E642A0A-BCCF-41DE-937D-8C8BE45F3AAC}" name="History_Covid"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}" name="Table7" displayName="Table7" ref="A1:D11" totalsRowShown="0">
+  <autoFilter ref="A1:D11" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{82F6FD84-E924-495D-9C8C-D8D902D02007}" name="Column Name"/>
+    <tableColumn id="2" xr3:uid="{9EB30155-F8F4-4911-9394-0E8B659DAAA6}" name="Type"/>
+    <tableColumn id="3" xr3:uid="{9D75EC3A-EE92-4C84-BF2B-9B7C70902EF5}" name="Key"/>
+    <tableColumn id="4" xr3:uid="{EB200C63-6CF0-430C-A0F9-513995D48DCB}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2614,7 +2685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6223762B-2B63-423A-B0E8-AA47018227CA}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -2682,7 +2753,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2870,11 +2941,263 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D2BEAD-878D-4C61-B4B1-129D00085AAC}">
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>219</v>
+      </c>
+      <c r="I4" t="s">
+        <v>212</v>
+      </c>
+      <c r="J4" t="s">
+        <v>198</v>
+      </c>
+      <c r="K4" t="s">
+        <v>213</v>
+      </c>
+      <c r="L4" t="s">
+        <v>214</v>
+      </c>
+      <c r="M4" t="s">
+        <v>215</v>
+      </c>
+      <c r="N4" t="s">
+        <v>216</v>
+      </c>
+      <c r="O4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>220</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4">
+        <v>43823</v>
+      </c>
+      <c r="K5">
+        <v>24</v>
+      </c>
+      <c r="L5">
+        <v>12</v>
+      </c>
+      <c r="M5">
+        <v>2019</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>221</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6" s="4">
+        <v>43933</v>
+      </c>
+      <c r="K6">
+        <v>12</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>2020</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>222</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7" s="4">
+        <v>44290</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>2021</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>219</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8" s="4">
+        <v>44291</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <v>2021</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9" s="4">
+        <v>44292</v>
+      </c>
+      <c r="K9">
+        <v>6</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <v>2021</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DB1A5A-DDCB-4891-AFE3-44BA495796A4}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2887,18 +3210,19 @@
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
+    <col min="17" max="17" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2912,7 +3236,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2926,7 +3250,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2940,7 +3264,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2954,31 +3278,34 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="B5" t="s">
         <v>199</v>
       </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
       <c r="D5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -2986,37 +3313,10 @@
       <c r="D7" t="s">
         <v>186</v>
       </c>
-      <c r="F7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" t="s">
-        <v>198</v>
-      </c>
-      <c r="J7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K7" t="s">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
-      </c>
-      <c r="L7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M7" t="s">
-        <v>11</v>
-      </c>
-      <c r="N7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -3025,36 +3325,39 @@
         <v>186</v>
       </c>
       <c r="F8" t="s">
-        <v>178</v>
+        <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>167</v>
+        <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>201</v>
-      </c>
-      <c r="J8">
-        <v>70</v>
-      </c>
-      <c r="K8">
-        <v>24</v>
-      </c>
-      <c r="L8">
-        <v>100</v>
-      </c>
-      <c r="M8">
-        <v>100</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="J8" t="s">
+        <v>198</v>
+      </c>
+      <c r="K8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -3063,36 +3366,39 @@
         <v>186</v>
       </c>
       <c r="F9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G9" t="s">
         <v>131</v>
       </c>
       <c r="H9" t="s">
-        <v>168</v>
-      </c>
-      <c r="I9" t="s">
-        <v>202</v>
-      </c>
-      <c r="J9">
+        <v>167</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="K9">
         <v>70</v>
       </c>
-      <c r="K9">
-        <v>25</v>
-      </c>
       <c r="L9">
-        <v>130</v>
+        <v>24</v>
       </c>
       <c r="M9">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="N9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -3101,107 +3407,160 @@
         <v>186</v>
       </c>
       <c r="F10" t="s">
+        <v>179</v>
+      </c>
+      <c r="G10" t="s">
+        <v>131</v>
+      </c>
+      <c r="H10" t="s">
+        <v>168</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="K10">
+        <v>70</v>
+      </c>
+      <c r="L10">
+        <v>25</v>
+      </c>
+      <c r="M10">
+        <v>130</v>
+      </c>
+      <c r="N10">
+        <v>129</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>186</v>
+      </c>
+      <c r="F11" t="s">
         <v>180</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G11" t="s">
         <v>132</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
         <v>169</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I11">
+        <v>6</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="J10">
+      <c r="K11">
         <v>70</v>
       </c>
-      <c r="K10">
+      <c r="L11">
         <v>36</v>
       </c>
-      <c r="L10">
+      <c r="M11">
         <v>140</v>
       </c>
-      <c r="M10">
+      <c r="N11">
         <v>198</v>
       </c>
-      <c r="N10">
+      <c r="O11">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
         <v>181</v>
-      </c>
-      <c r="G11" t="s">
-        <v>133</v>
-      </c>
-      <c r="H11" t="s">
-        <v>170</v>
-      </c>
-      <c r="I11" t="s">
-        <v>201</v>
-      </c>
-      <c r="J11">
-        <v>70</v>
-      </c>
-      <c r="K11">
-        <v>27</v>
-      </c>
-      <c r="L11">
-        <v>146</v>
-      </c>
-      <c r="M11">
-        <v>200</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>182</v>
       </c>
       <c r="G12" t="s">
         <v>133</v>
       </c>
       <c r="H12" t="s">
-        <v>171</v>
-      </c>
-      <c r="I12" t="s">
-        <v>202</v>
-      </c>
-      <c r="J12">
+        <v>170</v>
+      </c>
+      <c r="I12">
+        <v>200</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="K12">
         <v>70</v>
       </c>
-      <c r="K12">
-        <v>48</v>
-      </c>
       <c r="L12">
+        <v>27</v>
+      </c>
+      <c r="M12">
+        <v>146</v>
+      </c>
+      <c r="N12">
         <v>200</v>
       </c>
-      <c r="M12">
-        <v>141</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G13" t="s">
         <v>133</v>
       </c>
       <c r="H13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I13">
+        <v>400</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="K13">
+        <v>70</v>
+      </c>
+      <c r="L13">
+        <v>48</v>
+      </c>
+      <c r="M13">
+        <v>200</v>
+      </c>
+      <c r="N13">
+        <v>141</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>183</v>
+      </c>
+      <c r="G14" t="s">
+        <v>133</v>
+      </c>
+      <c r="H14" t="s">
         <v>172</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I14">
+        <v>4500</v>
+      </c>
+      <c r="J14" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
         <v>203</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Desc and Model.
- Recreate model from Warehouse to Database.
- Create Medical_Detail table.
- Delete Diagnosis_ID from Medical table.
- Fix Medical table and Date_Time table.
- Delete Diagnosis table.
- Keep tables: Disease, Symptom, Insurance, Patient.
</commit_message>
<xml_diff>
--- a/docs/Desc and Example Tables.xlsx
+++ b/docs/Desc and Example Tables.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17737\Desktop\FPT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17737\Desktop\FPT\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDE5887-9BA6-4987-9514-2107B8106FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170E2D92-DDDA-4143-8388-A7017370CFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{76F2D5F5-96DF-42B7-9620-589D1FA50423}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{76F2D5F5-96DF-42B7-9620-589D1FA50423}"/>
   </bookViews>
   <sheets>
     <sheet name="Insurance" sheetId="2" r:id="rId1"/>
     <sheet name="Patient" sheetId="4" r:id="rId2"/>
     <sheet name="Disease" sheetId="5" r:id="rId3"/>
     <sheet name="Symptom" sheetId="6" r:id="rId4"/>
-    <sheet name="Diagnosis" sheetId="7" r:id="rId5"/>
-    <sheet name="Date" sheetId="8" r:id="rId6"/>
+    <sheet name="Medical Detail" sheetId="9" r:id="rId5"/>
+    <sheet name="Date_Time" sheetId="8" r:id="rId6"/>
     <sheet name="Medical" sheetId="1" r:id="rId7"/>
+    <sheet name="FACT " sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="243">
   <si>
     <t>Medical_ID</t>
   </si>
@@ -54,9 +55,6 @@
     <t>History_Covid</t>
   </si>
   <si>
-    <t>Patient_Weight</t>
-  </si>
-  <si>
     <t>Patient_Age</t>
   </si>
   <si>
@@ -159,9 +157,6 @@
     <t>Use Table</t>
   </si>
   <si>
-    <t>Symtom_ID</t>
-  </si>
-  <si>
     <t>Symtom_Name</t>
   </si>
   <si>
@@ -390,15 +385,6 @@
     <t>Having one or two of the symptoms does not mean you have lung cancer</t>
   </si>
   <si>
-    <t>Symtom_Repeated_Time</t>
-  </si>
-  <si>
-    <t>Probability_Diagnosis</t>
-  </si>
-  <si>
-    <t>Random var</t>
-  </si>
-  <si>
     <t>Patient_Name</t>
   </si>
   <si>
@@ -534,15 +520,9 @@
     <t>Matching HMO = 6k, PMO = 9k</t>
   </si>
   <si>
-    <t>DA1-DA5000</t>
-  </si>
-  <si>
     <t>(S1-S32)</t>
   </si>
   <si>
-    <t>random(S1-S32)</t>
-  </si>
-  <si>
     <t>DA1</t>
   </si>
   <si>
@@ -561,18 +541,9 @@
     <t>DA6</t>
   </si>
   <si>
-    <t>DA7</t>
-  </si>
-  <si>
-    <t>DA8</t>
-  </si>
-  <si>
     <t>M1-M5000</t>
   </si>
   <si>
-    <t>random DA1-5000</t>
-  </si>
-  <si>
     <t>random P1-P1000 (5000 lần)</t>
   </si>
   <si>
@@ -600,12 +571,6 @@
     <t>I2005</t>
   </si>
   <si>
-    <t>Theo bảng Patient(base on P_ID)</t>
-  </si>
-  <si>
-    <t>Total: 5000 colums</t>
-  </si>
-  <si>
     <t>Total: 32 columns</t>
   </si>
   <si>
@@ -627,9 +592,6 @@
     <t>Symptom_Stage_Desc</t>
   </si>
   <si>
-    <t>Symptom_Repeated_Time</t>
-  </si>
-  <si>
     <t>Random (I2000-I3000)</t>
   </si>
   <si>
@@ -672,9 +634,6 @@
     <t>Blodd_Sugar_mgdL</t>
   </si>
   <si>
-    <t>Random(5000 times) (Year between 2019 -2021)</t>
-  </si>
-  <si>
     <t>Column</t>
   </si>
   <si>
@@ -696,9 +655,6 @@
     <t>Day_Of_Week</t>
   </si>
   <si>
-    <t>DT(1-5000)</t>
-  </si>
-  <si>
     <t>Day base on Appoiment_Date</t>
   </si>
   <si>
@@ -711,20 +667,116 @@
     <t>Base on Month(1-&gt;3 = 3 -&gt; 6 =2,.. 9 -&gt; 12 = 4)</t>
   </si>
   <si>
-    <t>use format Month-Day-Year</t>
-  </si>
-  <si>
-    <t>Random DT(1-5000)</t>
-  </si>
-  <si>
-    <t>Theo bảng Date(base on Date_ID)</t>
+    <t>Spouse_Occupation</t>
+  </si>
+  <si>
+    <t>Spouse_Name</t>
+  </si>
+  <si>
+    <t>Same with Medical Table</t>
+  </si>
+  <si>
+    <t>random name</t>
+  </si>
+  <si>
+    <t>random phone number</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>Doctor_Name</t>
+  </si>
+  <si>
+    <t>Allergies</t>
+  </si>
+  <si>
+    <t>random  1, 0</t>
+  </si>
+  <si>
+    <t>Work_Phone</t>
+  </si>
+  <si>
+    <t>M100</t>
+  </si>
+  <si>
+    <t>M201</t>
+  </si>
+  <si>
+    <t>M345</t>
+  </si>
+  <si>
+    <t>M4567</t>
+  </si>
+  <si>
+    <t>Surgery_Status</t>
+  </si>
+  <si>
+    <t>Spouse_Phone</t>
+  </si>
+  <si>
+    <t>Social_Security_Last_4</t>
+  </si>
+  <si>
+    <t>Random name</t>
+  </si>
+  <si>
+    <t>Random phone</t>
+  </si>
+  <si>
+    <t>Random occupation</t>
+  </si>
+  <si>
+    <t>Random 4 number</t>
+  </si>
+  <si>
+    <t>Same with Symptom_ID</t>
+  </si>
+  <si>
+    <t>Random Appointment_Date(based Date_Time table)</t>
+  </si>
+  <si>
+    <t>Random 1,0</t>
+  </si>
+  <si>
+    <t>Random date(2000 times unique)</t>
+  </si>
+  <si>
+    <t>5000 Colums</t>
+  </si>
+  <si>
+    <t>2000 colums</t>
+  </si>
+  <si>
+    <t>Column_Name</t>
+  </si>
+  <si>
+    <t>Social_Sercurity_Last_4</t>
+  </si>
+  <si>
+    <t>Patient_BloodType</t>
+  </si>
+  <si>
+    <t>Symtom_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -745,8 +797,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -759,8 +819,14 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -781,11 +847,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -796,16 +886,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -828,25 +990,6 @@
     <tableColumn id="2" xr3:uid="{43A7CF1E-6DA7-42A6-BB3C-7375AFBFC8EC}" name="Insurance_Cover_Ammount"/>
     <tableColumn id="3" xr3:uid="{35421352-61FA-438F-8AF4-BCEFA7F89966}" name="Insurance_Type"/>
     <tableColumn id="4" xr3:uid="{57F3944B-545F-44A1-BAED-610981CC9597}" name="Insurance_Expired"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}" name="Table14" displayName="Table14" ref="F8:O14" totalsRowShown="0">
-  <autoFilter ref="F8:O14" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{7227021B-20F6-4823-AE83-785A5D6E3F88}" name="Medical_ID"/>
-    <tableColumn id="2" xr3:uid="{64B431FB-56E7-42B2-A897-6C2F79451140}" name="Patient_ID"/>
-    <tableColumn id="3" xr3:uid="{CF43519C-595E-44E5-8532-18F6EFF0E066}" name="Diagnosis_ID"/>
-    <tableColumn id="7" xr3:uid="{E8BE27C5-42CD-4730-BA30-99000F8955AF}" name="Date_ID"/>
-    <tableColumn id="4" xr3:uid="{FABB793E-D151-4EA0-BE4C-09A512CB3310}" name="Appointment_Date" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{63B02EB5-8B62-4692-91B0-6C39B73E5A76}" name="Patient_Weight"/>
-    <tableColumn id="10" xr3:uid="{569B60D3-E99F-4244-98FD-6901E280C441}" name="Patient_Age"/>
-    <tableColumn id="11" xr3:uid="{1BC26F58-90ED-470B-8A35-E77C28D767B4}" name="Blood_Pressure_mmHg"/>
-    <tableColumn id="12" xr3:uid="{E301E0FD-788A-4E47-98FC-6BDFB2D5BF3D}" name="Blood_Sugar_mgdL"/>
-    <tableColumn id="5" xr3:uid="{9E642A0A-BCCF-41DE-937D-8C8BE45F3AAC}" name="History_Covid"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -914,38 +1057,26 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3D39A906-9290-4620-88D9-3D0E74A0723B}" name="Table6" displayName="Table6" ref="I5:M13" totalsRowShown="0">
-  <autoFilter ref="I5:M13" xr:uid="{3D39A906-9290-4620-88D9-3D0E74A0723B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E1C62383-673F-4915-8A77-C836FB2F6AB0}" name="Table8" displayName="Table8" ref="I7:M13" totalsRowShown="0">
+  <autoFilter ref="I7:M13" xr:uid="{E1C62383-673F-4915-8A77-C836FB2F6AB0}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8B92FE1E-E55E-4D2C-9DD5-FF786D76CF38}" name="Diagnosis_ID"/>
-    <tableColumn id="2" xr3:uid="{A00622D6-26D8-4327-8BDB-F4490C333D60}" name="Symptom_ID"/>
-    <tableColumn id="5" xr3:uid="{36988D2B-84DA-4DF0-9ABB-712017EB4C11}" name="Appointment_Date"/>
-    <tableColumn id="3" xr3:uid="{C12F9D53-8CEA-446C-925B-45B03D048F80}" name="Symtom_Repeated_Time"/>
-    <tableColumn id="4" xr3:uid="{E2BBC69F-57BF-44C4-B75E-BD7E94525595}" name="Probability_Diagnosis"/>
+    <tableColumn id="1" xr3:uid="{8D5FF6E7-EDC8-4524-83B9-C3603063E85C}" name="Medical_ID" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{8C1582DA-E5CC-4883-958F-C05675AAE307}" name="Diagnosis_ID" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{544D9204-7114-44F9-8E23-6083FCB6C6E6}" name="Spouse_Name"/>
+    <tableColumn id="4" xr3:uid="{BE48A60E-D0F7-48CE-9B08-8E3912CD1C5D}" name="Allergies"/>
+    <tableColumn id="5" xr3:uid="{B2F77CBF-8B46-4897-B2C8-CC185D951354}" name="Work_Phone"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{02A19413-FB07-4759-A25F-021BF1EB9D67}" name="Table9" displayName="Table9" ref="A1:D6" totalsRowShown="0">
-  <autoFilter ref="A1:D6" xr:uid="{02A19413-FB07-4759-A25F-021BF1EB9D67}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C62703B6-F26D-4EE6-A104-1EA4B7BFB8C2}" name="Column Name"/>
-    <tableColumn id="2" xr3:uid="{E783E5B4-4EFB-4973-B0C1-57515A5A1856}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{481B3B18-84BD-4AC1-BF70-8728E6987868}" name="Key"/>
-    <tableColumn id="4" xr3:uid="{D2E9C8B3-3953-485C-A08D-AE11E25EB92C}" name="Note"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8D386086-412F-4F15-B57A-3524CD3A74AA}" name="Table3" displayName="Table3" ref="I4:O9" totalsRowShown="0">
-  <autoFilter ref="I4:O9" xr:uid="{8D386086-412F-4F15-B57A-3524CD3A74AA}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8D386086-412F-4F15-B57A-3524CD3A74AA}" name="Table3" displayName="Table3" ref="I3:P8" totalsRowShown="0">
+  <autoFilter ref="I3:P8" xr:uid="{8D386086-412F-4F15-B57A-3524CD3A74AA}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{A202697D-1FEA-4478-A5FB-08AD456971F0}" name="Date_ID"/>
-    <tableColumn id="2" xr3:uid="{D24A4C43-A5DC-409B-BAB6-D3A7D35C28F3}" name="Appointment_Date" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{DA482D08-78D6-44CC-9ED0-76B2D28AF51C}" name="Medical_ID"/>
+    <tableColumn id="2" xr3:uid="{D24A4C43-A5DC-409B-BAB6-D3A7D35C28F3}" name="Appointment_Date" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{B9B3969D-11B2-401B-B112-79537FC98542}" name="Day"/>
     <tableColumn id="4" xr3:uid="{E91D160C-CEF2-468E-B92F-85F7541A1661}" name="Month"/>
     <tableColumn id="5" xr3:uid="{1862BDC0-7D95-41DE-A1A2-B187644035A7}" name="Year"/>
@@ -956,14 +1087,30 @@
 </table>
 </file>
 
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}" name="Table7" displayName="Table7" ref="A1:D11" totalsRowShown="0">
-  <autoFilter ref="A1:D11" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}"/>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}" name="Table7" displayName="Table7" ref="A1:D9" totalsRowShown="0">
+  <autoFilter ref="A1:D9" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{82F6FD84-E924-495D-9C8C-D8D902D02007}" name="Column Name"/>
     <tableColumn id="2" xr3:uid="{9EB30155-F8F4-4911-9394-0E8B659DAAA6}" name="Type"/>
     <tableColumn id="3" xr3:uid="{9D75EC3A-EE92-4C84-BF2B-9B7C70902EF5}" name="Key"/>
     <tableColumn id="4" xr3:uid="{EB200C63-6CF0-430C-A0F9-513995D48DCB}" name="Note"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}" name="Table14" displayName="Table14" ref="G7:M13" totalsRowShown="0">
+  <autoFilter ref="G7:M13" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{7227021B-20F6-4823-AE83-785A5D6E3F88}" name="Medical_ID"/>
+    <tableColumn id="2" xr3:uid="{64B431FB-56E7-42B2-A897-6C2F79451140}" name="Patient_ID"/>
+    <tableColumn id="7" xr3:uid="{E8BE27C5-42CD-4730-BA30-99000F8955AF}" name="Appointment_Date" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{FABB793E-D151-4EA0-BE4C-09A512CB3310}" name="Spouse_Name" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{63B02EB5-8B62-4692-91B0-6C39B73E5A76}" name="Spouse_Phone"/>
+    <tableColumn id="10" xr3:uid="{569B60D3-E99F-4244-98FD-6901E280C441}" name="Spouse_Occupation"/>
+    <tableColumn id="11" xr3:uid="{1BC26F58-90ED-470B-8A35-E77C28D767B4}" name="Social_Security_Last_4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1287,79 +1434,79 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" t="s">
         <v>158</v>
       </c>
-      <c r="E3" t="s">
-        <v>163</v>
-      </c>
       <c r="I3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="J3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="L3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="J4">
         <v>6000</v>
       </c>
       <c r="K4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="L4" s="2">
         <v>45295</v>
@@ -1367,36 +1514,36 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="I5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J5">
         <v>9000</v>
       </c>
       <c r="K5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I6" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="J6">
         <v>6000</v>
       </c>
       <c r="K6" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="L6" s="2">
         <v>45295</v>
@@ -1404,21 +1551,21 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="J7">
         <v>9000</v>
       </c>
       <c r="K7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1458,16 +1605,16 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1475,119 +1622,119 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I6" t="s">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="K6" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L6" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="M6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="O6" t="s">
+        <v>117</v>
+      </c>
+      <c r="P6" t="s">
         <v>122</v>
       </c>
-      <c r="P6" t="s">
-        <v>127</v>
-      </c>
       <c r="Q6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="R6" t="s">
         <v>3</v>
       </c>
       <c r="S6" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="T6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
         <v>121</v>
       </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="I7" t="s">
         <v>126</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
+        <v>148</v>
+      </c>
+      <c r="K7" t="s">
         <v>131</v>
       </c>
-      <c r="J7" t="s">
-        <v>153</v>
-      </c>
-      <c r="K7" t="s">
-        <v>136</v>
-      </c>
       <c r="L7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="M7">
         <v>23</v>
@@ -1596,10 +1743,10 @@
         <v>60601</v>
       </c>
       <c r="O7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="P7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="Q7">
         <v>70</v>
@@ -1616,25 +1763,25 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J8" t="s">
+        <v>175</v>
+      </c>
+      <c r="K8" t="s">
         <v>132</v>
       </c>
-      <c r="J8" t="s">
-        <v>185</v>
-      </c>
-      <c r="K8" t="s">
-        <v>137</v>
-      </c>
       <c r="L8" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="M8">
         <v>24</v>
@@ -1643,10 +1790,10 @@
         <v>60601</v>
       </c>
       <c r="O8" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="P8" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="Q8">
         <v>70</v>
@@ -1663,25 +1810,25 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
+        <v>123</v>
+      </c>
+      <c r="I9" t="s">
         <v>128</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
+        <v>184</v>
+      </c>
+      <c r="K9" t="s">
         <v>133</v>
       </c>
-      <c r="J9" t="s">
-        <v>197</v>
-      </c>
-      <c r="K9" t="s">
-        <v>138</v>
-      </c>
       <c r="L9" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="M9">
         <v>40</v>
@@ -1690,10 +1837,10 @@
         <v>60601</v>
       </c>
       <c r="O9" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="P9" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="Q9">
         <v>70</v>
@@ -1710,25 +1857,25 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>125</v>
+      </c>
+      <c r="I10" t="s">
         <v>129</v>
       </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>130</v>
-      </c>
-      <c r="I10" t="s">
-        <v>134</v>
-      </c>
       <c r="J10" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="K10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L10" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="M10">
         <v>79</v>
@@ -1737,10 +1884,10 @@
         <v>60601</v>
       </c>
       <c r="O10" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="P10" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="Q10">
         <v>70</v>
@@ -1760,22 +1907,22 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="I11" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="J11" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="K11" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="L11" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="M11">
         <v>80</v>
@@ -1784,10 +1931,10 @@
         <v>60601</v>
       </c>
       <c r="O11" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="P11" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="Q11">
         <v>70</v>
@@ -1804,29 +1951,29 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1843,7 +1990,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,144 +2009,144 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
         <v>15</v>
       </c>
-      <c r="J6" t="s">
-        <v>16</v>
-      </c>
       <c r="K6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" t="s">
         <v>30</v>
-      </c>
-      <c r="L8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" t="s">
         <v>32</v>
-      </c>
-      <c r="L9" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2015,8 +2162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9772A3FD-BEF1-40F4-9572-5D20CC2045A5}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,642 +2180,642 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="J6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" t="s">
         <v>40</v>
-      </c>
-      <c r="L6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" t="s">
         <v>18</v>
       </c>
-      <c r="I7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" t="s">
-        <v>19</v>
-      </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L7">
         <v>1</v>
       </c>
       <c r="M7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="M8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="I9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L9">
         <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L10">
         <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="I11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L11">
         <v>1</v>
       </c>
       <c r="M11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L12">
         <v>2</v>
       </c>
       <c r="M12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L13">
         <v>2</v>
       </c>
       <c r="M13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L14">
         <v>2</v>
       </c>
       <c r="M14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L15">
         <v>1</v>
       </c>
       <c r="M15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L16">
         <v>1</v>
       </c>
       <c r="M16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L17">
         <v>1</v>
       </c>
       <c r="M17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L18">
         <v>2</v>
       </c>
       <c r="M18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L19">
         <v>3</v>
       </c>
       <c r="M19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L20">
         <v>1</v>
       </c>
       <c r="M20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L21">
         <v>1</v>
       </c>
       <c r="M21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L22">
         <v>1</v>
       </c>
       <c r="M22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L23">
         <v>2</v>
       </c>
       <c r="M23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L24">
         <v>3</v>
       </c>
       <c r="M24" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L25">
         <v>3</v>
       </c>
       <c r="M25" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L26">
         <v>3</v>
       </c>
       <c r="M26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L27">
         <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L28">
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L29">
         <v>1</v>
       </c>
       <c r="M29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L30">
         <v>1</v>
       </c>
       <c r="M30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K31" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L31">
         <v>2</v>
       </c>
       <c r="M31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L32">
         <v>2</v>
       </c>
       <c r="M32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L33">
         <v>1</v>
       </c>
       <c r="M33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I34" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K34" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L34">
         <v>2</v>
       </c>
       <c r="M34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I35" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L35">
         <v>3</v>
       </c>
       <c r="M35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I36" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L36">
         <v>3</v>
       </c>
       <c r="M36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L37">
         <v>3</v>
       </c>
       <c r="M37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I38" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K38" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L38">
         <v>3</v>
       </c>
       <c r="M38" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2682,259 +2829,225 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6223762B-2B63-423A-B0E8-AA47018227CA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1D7C2F-E788-483F-92A0-7A826F78507E}">
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.42578125" customWidth="1"/>
-    <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="13" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
+      <c r="D1" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>164</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>166</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
-      </c>
-      <c r="I5" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" t="s">
-        <v>191</v>
-      </c>
-      <c r="K5" t="s">
-        <v>198</v>
-      </c>
-      <c r="L5" t="s">
-        <v>116</v>
-      </c>
-      <c r="M5" t="s">
-        <v>117</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>221</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
-      </c>
-      <c r="I6" t="s">
-        <v>167</v>
-      </c>
-      <c r="J6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" t="s">
-        <v>201</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>10</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>209</v>
+      </c>
+      <c r="L7" t="s">
+        <v>219</v>
+      </c>
+      <c r="M7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I8" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="J7" t="s">
-        <v>101</v>
-      </c>
-      <c r="K7" t="s">
-        <v>202</v>
-      </c>
-      <c r="L7">
-        <v>4</v>
-      </c>
-      <c r="M7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I8" t="s">
+      <c r="J8" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="K8" t="s">
+        <v>131</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>12345679</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I9" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="J8" t="s">
-        <v>54</v>
-      </c>
-      <c r="K8" t="s">
-        <v>202</v>
-      </c>
-      <c r="L8">
-        <v>5</v>
-      </c>
-      <c r="M8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>187</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="J9" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="K9" t="s">
+        <v>213</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>12345679</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I10" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="J9" t="s">
-        <v>55</v>
-      </c>
-      <c r="K9" t="s">
-        <v>201</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I10" t="s">
+      <c r="J10" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="K10" t="s">
+        <v>214</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>12345679</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I11" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="J10" t="s">
-        <v>56</v>
-      </c>
-      <c r="K10" t="s">
-        <v>202</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I11" t="s">
+      <c r="J11" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="K11" t="s">
+        <v>215</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>12345679</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>237</v>
+      </c>
+      <c r="I12" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="J11" t="s">
-        <v>57</v>
-      </c>
-      <c r="K11" t="s">
-        <v>201</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I12" t="s">
+      <c r="J12" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="K12" t="s">
+        <v>216</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>12345679</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I13" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="J12" t="s">
-        <v>58</v>
-      </c>
-      <c r="K12" t="s">
-        <v>202</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I13" t="s">
-        <v>174</v>
-      </c>
-      <c r="J13" t="s">
-        <v>59</v>
+      <c r="J13" s="10" t="s">
+        <v>165</v>
       </c>
       <c r="K13" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="L13">
         <v>1</v>
       </c>
       <c r="M13">
-        <v>10</v>
+        <v>12345679</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
-    <tablePart r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
@@ -2942,10 +3055,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D2BEAD-878D-4C61-B4B1-129D00085AAC}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2954,234 +3067,244 @@
     <col min="4" max="4" width="44" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
-    <col min="14" max="14" width="10" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" customWidth="1"/>
+    <col min="15" max="15" width="10" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D3" t="s">
+        <v>204</v>
+      </c>
+      <c r="I3" t="s">
+        <v>198</v>
+      </c>
+      <c r="J3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>185</v>
+      </c>
+      <c r="L3" t="s">
         <v>199</v>
       </c>
-      <c r="C2" t="s">
+      <c r="M3" t="s">
+        <v>200</v>
+      </c>
+      <c r="N3" t="s">
+        <v>201</v>
+      </c>
+      <c r="O3" t="s">
+        <v>202</v>
+      </c>
+      <c r="P3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>205</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>168</v>
+      </c>
+      <c r="K4" s="4">
+        <v>43823</v>
+      </c>
+      <c r="L4">
+        <v>24</v>
+      </c>
+      <c r="M4">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>198</v>
-      </c>
-      <c r="B3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>213</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>219</v>
-      </c>
-      <c r="I4" t="s">
-        <v>212</v>
-      </c>
-      <c r="J4" t="s">
-        <v>198</v>
-      </c>
-      <c r="K4" t="s">
-        <v>213</v>
-      </c>
-      <c r="L4" t="s">
-        <v>214</v>
-      </c>
-      <c r="M4" t="s">
-        <v>215</v>
-      </c>
-      <c r="N4" t="s">
-        <v>216</v>
-      </c>
-      <c r="O4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>2019</v>
+      </c>
+      <c r="O4">
+        <v>4</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5" s="4">
-        <v>43823</v>
-      </c>
-      <c r="K5">
-        <v>24</v>
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>222</v>
+      </c>
+      <c r="K5" s="4">
+        <v>43933</v>
       </c>
       <c r="L5">
         <v>12</v>
       </c>
       <c r="M5">
-        <v>2019</v>
+        <v>4</v>
       </c>
       <c r="N5">
-        <v>4</v>
+        <v>2020</v>
       </c>
       <c r="O5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="I6">
-        <v>2</v>
-      </c>
-      <c r="J6" s="4">
-        <v>43933</v>
-      </c>
-      <c r="K6">
-        <v>12</v>
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>223</v>
+      </c>
+      <c r="K6" s="4">
+        <v>44290</v>
       </c>
       <c r="L6">
         <v>4</v>
       </c>
       <c r="M6">
-        <v>2020</v>
+        <v>4</v>
       </c>
       <c r="N6">
-        <v>2</v>
+        <v>2021</v>
       </c>
       <c r="O6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="I7">
-        <v>3</v>
-      </c>
-      <c r="J7" s="4">
-        <v>44290</v>
-      </c>
-      <c r="K7">
         <v>4</v>
       </c>
+      <c r="J7" t="s">
+        <v>224</v>
+      </c>
+      <c r="K7" s="4">
+        <v>44291</v>
+      </c>
       <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="M7">
         <v>4</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>2021</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>2</v>
       </c>
-      <c r="O7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>217</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>219</v>
-      </c>
+      <c r="P7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8" t="s">
+        <v>225</v>
+      </c>
+      <c r="K8" s="4">
+        <v>44292</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="M8">
         <v>4</v>
       </c>
-      <c r="J8" s="4">
-        <v>44291</v>
-      </c>
-      <c r="K8">
+      <c r="N8">
+        <v>2021</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8">
         <v>5</v>
       </c>
-      <c r="L8">
-        <v>4</v>
-      </c>
-      <c r="M8">
-        <v>2021</v>
-      </c>
-      <c r="N8">
-        <v>2</v>
-      </c>
-      <c r="O8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I9">
-        <v>5</v>
-      </c>
-      <c r="J9" s="4">
-        <v>44292</v>
-      </c>
-      <c r="K9">
-        <v>6</v>
-      </c>
-      <c r="L9">
-        <v>4</v>
-      </c>
-      <c r="M9">
-        <v>2021</v>
-      </c>
-      <c r="N9">
-        <v>2</v>
-      </c>
-      <c r="O9">
-        <v>5</v>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -3194,10 +3317,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DB1A5A-DDCB-4891-AFE3-44BA495796A4}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3222,346 +3345,264 @@
     <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>186</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>208</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>231</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>185</v>
+      </c>
+      <c r="J7" t="s">
+        <v>209</v>
+      </c>
+      <c r="K7" t="s">
+        <v>227</v>
+      </c>
+      <c r="L7" t="s">
+        <v>208</v>
+      </c>
+      <c r="M7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>232</v>
+      </c>
+      <c r="G8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H8" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K8">
+        <v>24</v>
+      </c>
+      <c r="L8">
+        <v>100</v>
+      </c>
+      <c r="M8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>226</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>235</v>
+      </c>
+      <c r="G9" t="s">
+        <v>169</v>
+      </c>
+      <c r="H9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K9">
+        <v>25</v>
+      </c>
+      <c r="L9">
+        <v>130</v>
+      </c>
+      <c r="M9">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>170</v>
+      </c>
+      <c r="H10" t="s">
+        <v>127</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K10">
+        <v>36</v>
+      </c>
+      <c r="L10">
+        <v>140</v>
+      </c>
+      <c r="M10">
         <v>198</v>
       </c>
-      <c r="B6" t="s">
-        <v>199</v>
-      </c>
-      <c r="D6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>186</v>
-      </c>
-      <c r="F8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" t="s">
-        <v>212</v>
-      </c>
-      <c r="J8" t="s">
-        <v>198</v>
-      </c>
-      <c r="K8" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" t="s">
-        <v>5</v>
-      </c>
-      <c r="M8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N8" t="s">
-        <v>11</v>
-      </c>
-      <c r="O8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F9" t="s">
-        <v>178</v>
-      </c>
-      <c r="G9" t="s">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>171</v>
+      </c>
+      <c r="H11" t="s">
+        <v>128</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="H9" t="s">
-        <v>167</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="K9">
-        <v>70</v>
-      </c>
-      <c r="L9">
-        <v>24</v>
-      </c>
-      <c r="M9">
-        <v>100</v>
-      </c>
-      <c r="N9">
-        <v>100</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>186</v>
-      </c>
-      <c r="F10" t="s">
-        <v>179</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="K11">
+        <v>27</v>
+      </c>
+      <c r="L11">
+        <v>146</v>
+      </c>
+      <c r="M11">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>172</v>
+      </c>
+      <c r="H12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="H10" t="s">
-        <v>168</v>
-      </c>
-      <c r="I10">
-        <v>4</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="K10">
-        <v>70</v>
-      </c>
-      <c r="L10">
-        <v>25</v>
-      </c>
-      <c r="M10">
-        <v>130</v>
-      </c>
-      <c r="N10">
-        <v>129</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>186</v>
-      </c>
-      <c r="F11" t="s">
-        <v>180</v>
-      </c>
-      <c r="G11" t="s">
-        <v>132</v>
-      </c>
-      <c r="H11" t="s">
-        <v>169</v>
-      </c>
-      <c r="I11">
-        <v>6</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="K11">
-        <v>70</v>
-      </c>
-      <c r="L11">
-        <v>36</v>
-      </c>
-      <c r="M11">
-        <v>140</v>
-      </c>
-      <c r="N11">
-        <v>198</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>181</v>
-      </c>
-      <c r="G12" t="s">
-        <v>133</v>
-      </c>
-      <c r="H12" t="s">
-        <v>170</v>
-      </c>
-      <c r="I12">
+      <c r="K12">
+        <v>48</v>
+      </c>
+      <c r="L12">
         <v>200</v>
       </c>
-      <c r="J12" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="K12">
-        <v>70</v>
-      </c>
-      <c r="L12">
-        <v>27</v>
-      </c>
       <c r="M12">
-        <v>146</v>
-      </c>
-      <c r="N12">
-        <v>200</v>
-      </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
-        <v>182</v>
-      </c>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
-        <v>133</v>
+        <v>173</v>
       </c>
       <c r="H13" t="s">
-        <v>171</v>
-      </c>
-      <c r="I13">
-        <v>400</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="K13">
-        <v>70</v>
-      </c>
-      <c r="L13">
-        <v>48</v>
-      </c>
-      <c r="M13">
-        <v>200</v>
-      </c>
-      <c r="N13">
-        <v>141</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
-        <v>183</v>
-      </c>
-      <c r="G14" t="s">
-        <v>133</v>
-      </c>
-      <c r="H14" t="s">
-        <v>172</v>
-      </c>
-      <c r="I14">
-        <v>4500</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>203</v>
+        <v>128</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -3572,4 +3613,87 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96AE23BC-D532-4D1D-89E1-E9FF10131B02}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed init_mssql to fit staging. Added py_requirements
</commit_message>
<xml_diff>
--- a/docs/Desc and Example Tables.xlsx
+++ b/docs/Desc and Example Tables.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17737\Desktop\FPT\Project 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hungnguyen/Documents/FPT/Training/Project02/Healthcare-Group-02/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170E2D92-DDDA-4143-8388-A7017370CFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BE31DE-2455-8E49-A818-5FECB8ED3744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{76F2D5F5-96DF-42B7-9620-589D1FA50423}"/>
+    <workbookView xWindow="-120" yWindow="500" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{76F2D5F5-96DF-42B7-9620-589D1FA50423}"/>
   </bookViews>
   <sheets>
     <sheet name="Insurance" sheetId="2" r:id="rId1"/>
-    <sheet name="Patient" sheetId="4" r:id="rId2"/>
-    <sheet name="Disease" sheetId="5" r:id="rId3"/>
-    <sheet name="Symptom" sheetId="6" r:id="rId4"/>
-    <sheet name="Medical Detail" sheetId="9" r:id="rId5"/>
-    <sheet name="Date_Time" sheetId="8" r:id="rId6"/>
-    <sheet name="Medical" sheetId="1" r:id="rId7"/>
+    <sheet name="Disease" sheetId="5" r:id="rId2"/>
+    <sheet name="Medical" sheetId="1" r:id="rId3"/>
+    <sheet name="Medical Detail" sheetId="9" r:id="rId4"/>
+    <sheet name="Patient" sheetId="4" r:id="rId5"/>
+    <sheet name="Symptom" sheetId="6" r:id="rId6"/>
+    <sheet name="Date_Time" sheetId="8" r:id="rId7"/>
     <sheet name="FACT " sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="244">
   <si>
     <t>Medical_ID</t>
   </si>
@@ -770,6 +770,9 @@
   </si>
   <si>
     <t>Symtom_name</t>
+  </si>
+  <si>
+    <t>varchar</t>
   </si>
 </sst>
 </file>
@@ -903,7 +906,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -996,6 +999,62 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1BF5BAA7-47F9-4C06-8533-2B4A8BB67E63}" name="Table1" displayName="Table1" ref="I6:L11" totalsRowShown="0">
+  <autoFilter ref="I6:L11" xr:uid="{1BF5BAA7-47F9-4C06-8533-2B4A8BB67E63}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{615D9AEA-0A62-45B3-8C3F-B2E207F2FE15}" name="Disease_ID"/>
+    <tableColumn id="2" xr3:uid="{65553CDA-7889-4906-9077-CE29E5E9F108}" name="Disease_Name"/>
+    <tableColumn id="3" xr3:uid="{7A7F65A5-D854-4E93-8F57-B6AB731F5217}" name="Blood_Pressure_mmHg"/>
+    <tableColumn id="4" xr3:uid="{93FDDACE-8A10-4B23-A240-F8C77E138DD0}" name="Blood_Sugar_mgdL"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}" name="Table7" displayName="Table7" ref="A1:D9" totalsRowShown="0">
+  <autoFilter ref="A1:D9" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{82F6FD84-E924-495D-9C8C-D8D902D02007}" name="Column Name"/>
+    <tableColumn id="2" xr3:uid="{9EB30155-F8F4-4911-9394-0E8B659DAAA6}" name="Type"/>
+    <tableColumn id="3" xr3:uid="{9D75EC3A-EE92-4C84-BF2B-9B7C70902EF5}" name="Key"/>
+    <tableColumn id="4" xr3:uid="{EB200C63-6CF0-430C-A0F9-513995D48DCB}" name="Note"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}" name="Table14" displayName="Table14" ref="G7:M13" totalsRowShown="0">
+  <autoFilter ref="G7:M13" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{7227021B-20F6-4823-AE83-785A5D6E3F88}" name="Medical_ID"/>
+    <tableColumn id="2" xr3:uid="{64B431FB-56E7-42B2-A897-6C2F79451140}" name="Patient_ID"/>
+    <tableColumn id="7" xr3:uid="{E8BE27C5-42CD-4730-BA30-99000F8955AF}" name="Appointment_Date" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{FABB793E-D151-4EA0-BE4C-09A512CB3310}" name="Spouse_Name" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{63B02EB5-8B62-4692-91B0-6C39B73E5A76}" name="Spouse_Phone"/>
+    <tableColumn id="10" xr3:uid="{569B60D3-E99F-4244-98FD-6901E280C441}" name="Spouse_Occupation"/>
+    <tableColumn id="11" xr3:uid="{1BC26F58-90ED-470B-8A35-E77C28D767B4}" name="Social_Security_Last_4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E1C62383-673F-4915-8A77-C836FB2F6AB0}" name="Table8" displayName="Table8" ref="I7:M13" totalsRowShown="0">
+  <autoFilter ref="I7:M13" xr:uid="{E1C62383-673F-4915-8A77-C836FB2F6AB0}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{8D5FF6E7-EDC8-4524-83B9-C3603063E85C}" name="Medical_ID" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{8C1582DA-E5CC-4883-958F-C05675AAE307}" name="Diagnosis_ID" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{544D9204-7114-44F9-8E23-6083FCB6C6E6}" name="Spouse_Name"/>
+    <tableColumn id="4" xr3:uid="{BE48A60E-D0F7-48CE-9B08-8E3912CD1C5D}" name="Allergies"/>
+    <tableColumn id="5" xr3:uid="{B2F77CBF-8B46-4897-B2C8-CC185D951354}" name="Work_Phone"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F74E800A-84A7-412D-A3FF-DF9CA2CACD42}" name="Table4" displayName="Table4" ref="I6:T11" totalsRowShown="0">
   <autoFilter ref="I6:T11" xr:uid="{F74E800A-84A7-412D-A3FF-DF9CA2CACD42}"/>
   <tableColumns count="12">
@@ -1016,20 +1075,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1BF5BAA7-47F9-4C06-8533-2B4A8BB67E63}" name="Table1" displayName="Table1" ref="I6:L11" totalsRowShown="0">
-  <autoFilter ref="I6:L11" xr:uid="{1BF5BAA7-47F9-4C06-8533-2B4A8BB67E63}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{615D9AEA-0A62-45B3-8C3F-B2E207F2FE15}" name="Disease_ID"/>
-    <tableColumn id="2" xr3:uid="{65553CDA-7889-4906-9077-CE29E5E9F108}" name="Disease_Name"/>
-    <tableColumn id="3" xr3:uid="{7A7F65A5-D854-4E93-8F57-B6AB731F5217}" name="Blood_Pressure_mmHg"/>
-    <tableColumn id="4" xr3:uid="{93FDDACE-8A10-4B23-A240-F8C77E138DD0}" name="Blood_Sugar_mgdL"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E4C8AEE8-4517-4AA2-AA6B-380234F3FDBF}" name="Table2" displayName="Table2" ref="I6:M38" totalsRowShown="0">
   <autoFilter ref="I6:M38" xr:uid="{E4C8AEE8-4517-4AA2-AA6B-380234F3FDBF}"/>
   <tableColumns count="5">
@@ -1043,7 +1089,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{1911CEF0-3178-444A-AB4C-1FF818936319}" name="Table11" displayName="Table11" ref="A1:D7" totalsRowShown="0">
   <autoFilter ref="A1:D7" xr:uid="{1911CEF0-3178-444A-AB4C-1FF818936319}"/>
   <tableColumns count="4">
@@ -1056,21 +1102,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E1C62383-673F-4915-8A77-C836FB2F6AB0}" name="Table8" displayName="Table8" ref="I7:M13" totalsRowShown="0">
-  <autoFilter ref="I7:M13" xr:uid="{E1C62383-673F-4915-8A77-C836FB2F6AB0}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8D5FF6E7-EDC8-4524-83B9-C3603063E85C}" name="Medical_ID" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{8C1582DA-E5CC-4883-958F-C05675AAE307}" name="Diagnosis_ID" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{544D9204-7114-44F9-8E23-6083FCB6C6E6}" name="Spouse_Name"/>
-    <tableColumn id="4" xr3:uid="{BE48A60E-D0F7-48CE-9B08-8E3912CD1C5D}" name="Allergies"/>
-    <tableColumn id="5" xr3:uid="{B2F77CBF-8B46-4897-B2C8-CC185D951354}" name="Work_Phone"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8D386086-412F-4F15-B57A-3524CD3A74AA}" name="Table3" displayName="Table3" ref="I3:P8" totalsRowShown="0">
   <autoFilter ref="I3:P8" xr:uid="{8D386086-412F-4F15-B57A-3524CD3A74AA}"/>
   <tableColumns count="8">
@@ -1082,35 +1114,6 @@
     <tableColumn id="5" xr3:uid="{1862BDC0-7D95-41DE-A1A2-B187644035A7}" name="Year"/>
     <tableColumn id="6" xr3:uid="{4F990E3D-CB8C-4D22-AB85-94E8893F531B}" name="Quarter"/>
     <tableColumn id="7" xr3:uid="{CDEA9271-8A42-4757-9C7A-0F971EA26F77}" name="Day_Of_Week"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}" name="Table7" displayName="Table7" ref="A1:D9" totalsRowShown="0">
-  <autoFilter ref="A1:D9" xr:uid="{B58D8926-98D7-46D7-8529-DB1E0C90C543}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{82F6FD84-E924-495D-9C8C-D8D902D02007}" name="Column Name"/>
-    <tableColumn id="2" xr3:uid="{9EB30155-F8F4-4911-9394-0E8B659DAAA6}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{9D75EC3A-EE92-4C84-BF2B-9B7C70902EF5}" name="Key"/>
-    <tableColumn id="4" xr3:uid="{EB200C63-6CF0-430C-A0F9-513995D48DCB}" name="Note"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}" name="Table14" displayName="Table14" ref="G7:M13" totalsRowShown="0">
-  <autoFilter ref="G7:M13" xr:uid="{D5F42A0B-2DE6-4D8C-911A-FFBEC92B0B85}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{7227021B-20F6-4823-AE83-785A5D6E3F88}" name="Medical_ID"/>
-    <tableColumn id="2" xr3:uid="{64B431FB-56E7-42B2-A897-6C2F79451140}" name="Patient_ID"/>
-    <tableColumn id="7" xr3:uid="{E8BE27C5-42CD-4730-BA30-99000F8955AF}" name="Appointment_Date" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{FABB793E-D151-4EA0-BE4C-09A512CB3310}" name="Spouse_Name" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{63B02EB5-8B62-4692-91B0-6C39B73E5A76}" name="Spouse_Phone"/>
-    <tableColumn id="10" xr3:uid="{569B60D3-E99F-4244-98FD-6901E280C441}" name="Spouse_Occupation"/>
-    <tableColumn id="11" xr3:uid="{1BC26F58-90ED-470B-8A35-E77C28D767B4}" name="Social_Security_Last_4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1416,23 +1419,23 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1446,7 +1449,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>142</v>
       </c>
@@ -1460,7 +1463,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>152</v>
       </c>
@@ -1486,7 +1489,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>143</v>
       </c>
@@ -1512,7 +1515,7 @@
         <v>45295</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>144</v>
       </c>
@@ -1535,7 +1538,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I6" t="s">
         <v>149</v>
       </c>
@@ -1549,7 +1552,7 @@
         <v>45295</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I7" t="s">
         <v>150</v>
       </c>
@@ -1563,7 +1566,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
         <v>178</v>
       </c>
@@ -1571,6 +1574,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -1578,32 +1582,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7AF1BA3-C17A-4D61-9274-54FCDF565A10}">
-  <dimension ref="A1:T16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8961B12-14C4-41F4-847F-48839C9A3E3E}">
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" customWidth="1"/>
-    <col min="16" max="16" width="19.7109375" customWidth="1"/>
-    <col min="17" max="17" width="20.140625" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1617,363 +1617,132 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
-      </c>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I6" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>142</v>
+        <v>15</v>
       </c>
       <c r="K6" t="s">
-        <v>114</v>
+        <v>28</v>
       </c>
       <c r="L6" t="s">
-        <v>115</v>
-      </c>
-      <c r="M6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N6" t="s">
-        <v>116</v>
-      </c>
-      <c r="O6" t="s">
-        <v>117</v>
-      </c>
-      <c r="P6" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>124</v>
-      </c>
-      <c r="R6" t="s">
-        <v>3</v>
-      </c>
-      <c r="S6" t="s">
-        <v>195</v>
-      </c>
-      <c r="T6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>121</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I7" t="s">
-        <v>126</v>
+        <v>18</v>
       </c>
       <c r="J7" t="s">
-        <v>148</v>
+        <v>24</v>
       </c>
       <c r="K7" t="s">
-        <v>131</v>
+        <v>30</v>
       </c>
       <c r="L7" t="s">
-        <v>135</v>
-      </c>
-      <c r="M7">
-        <v>23</v>
-      </c>
-      <c r="N7">
-        <v>60601</v>
-      </c>
-      <c r="O7" t="s">
-        <v>137</v>
-      </c>
-      <c r="P7" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q7">
-        <v>70</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>120</v>
-      </c>
-      <c r="T7">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>118</v>
-      </c>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I8" t="s">
-        <v>127</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>175</v>
+        <v>25</v>
       </c>
       <c r="K8" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="L8" t="s">
-        <v>135</v>
-      </c>
-      <c r="M8">
-        <v>24</v>
-      </c>
-      <c r="N8">
-        <v>60601</v>
-      </c>
-      <c r="O8" t="s">
-        <v>138</v>
-      </c>
-      <c r="P8" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q8">
-        <v>70</v>
-      </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-      <c r="S8">
-        <v>121</v>
-      </c>
-      <c r="T8">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>123</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>177</v>
       </c>
       <c r="I9" t="s">
-        <v>128</v>
+        <v>20</v>
       </c>
       <c r="J9" t="s">
-        <v>184</v>
+        <v>26</v>
       </c>
       <c r="K9" t="s">
-        <v>133</v>
+        <v>31</v>
       </c>
       <c r="L9" t="s">
-        <v>135</v>
-      </c>
-      <c r="M9">
-        <v>40</v>
-      </c>
-      <c r="N9">
-        <v>60601</v>
-      </c>
-      <c r="O9" t="s">
-        <v>139</v>
-      </c>
-      <c r="P9" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q9">
-        <v>70</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>122</v>
-      </c>
-      <c r="T9">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>125</v>
-      </c>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I10" t="s">
-        <v>129</v>
+        <v>21</v>
       </c>
       <c r="J10" t="s">
-        <v>174</v>
+        <v>90</v>
       </c>
       <c r="K10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="L10" t="s">
-        <v>136</v>
-      </c>
-      <c r="M10">
-        <v>79</v>
-      </c>
-      <c r="N10">
-        <v>60601</v>
-      </c>
-      <c r="O10" t="s">
-        <v>139</v>
-      </c>
-      <c r="P10" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q10">
-        <v>70</v>
-      </c>
-      <c r="R10">
-        <v>1</v>
-      </c>
-      <c r="S10">
-        <v>123</v>
-      </c>
-      <c r="T10">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>192</v>
-      </c>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I11" t="s">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="J11" t="s">
-        <v>175</v>
+        <v>27</v>
       </c>
       <c r="K11" t="s">
-        <v>134</v>
+        <v>31</v>
       </c>
       <c r="L11" t="s">
-        <v>136</v>
-      </c>
-      <c r="M11">
-        <v>80</v>
-      </c>
-      <c r="N11">
-        <v>60601</v>
-      </c>
-      <c r="O11" t="s">
-        <v>139</v>
-      </c>
-      <c r="P11" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q11">
-        <v>70</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>124</v>
-      </c>
-      <c r="T11">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>178</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1986,28 +1755,36 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8961B12-14C4-41F4-847F-48839C9A3E3E}">
-  <dimension ref="A1:L11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DB1A5A-DDCB-4891-AFE3-44BA495796A4}">
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
+    <col min="17" max="17" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2021,132 +1798,885 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="J3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>208</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>231</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>185</v>
+      </c>
+      <c r="J7" t="s">
+        <v>209</v>
+      </c>
+      <c r="K7" t="s">
+        <v>227</v>
+      </c>
+      <c r="L7" t="s">
+        <v>208</v>
+      </c>
+      <c r="M7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>232</v>
+      </c>
+      <c r="G8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H8" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K8">
+        <v>24</v>
+      </c>
+      <c r="L8">
+        <v>100</v>
+      </c>
+      <c r="M8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>226</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>235</v>
+      </c>
+      <c r="G9" t="s">
+        <v>169</v>
+      </c>
+      <c r="H9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K9">
+        <v>25</v>
+      </c>
+      <c r="L9">
+        <v>130</v>
+      </c>
+      <c r="M9">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>170</v>
+      </c>
+      <c r="H10" t="s">
+        <v>127</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K10">
+        <v>36</v>
+      </c>
+      <c r="L10">
+        <v>140</v>
+      </c>
+      <c r="M10">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>171</v>
+      </c>
+      <c r="H11" t="s">
+        <v>128</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K11">
+        <v>27</v>
+      </c>
+      <c r="L11">
+        <v>146</v>
+      </c>
+      <c r="M11">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>172</v>
+      </c>
+      <c r="H12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K12">
+        <v>48</v>
+      </c>
+      <c r="L12">
+        <v>200</v>
+      </c>
+      <c r="M12">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>173</v>
+      </c>
+      <c r="H13" t="s">
+        <v>128</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1D7C2F-E788-483F-92A0-7A826F78507E}">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" customWidth="1"/>
+    <col min="12" max="13" width="20.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>218</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>219</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>209</v>
+      </c>
+      <c r="L7" t="s">
+        <v>219</v>
+      </c>
+      <c r="M7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I8" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="K8" t="s">
+        <v>131</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>12345679</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I9" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="K9" t="s">
+        <v>213</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>12345679</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I10" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="K10" t="s">
+        <v>214</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>12345679</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I11" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="K11" t="s">
+        <v>215</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>12345679</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>237</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="K12" t="s">
+        <v>216</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>12345679</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I13" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="K13" t="s">
+        <v>217</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>12345679</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7AF1BA3-C17A-4D61-9274-54FCDF565A10}">
+  <dimension ref="A1:T16"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" customWidth="1"/>
+    <col min="16" max="16" width="19.6640625" customWidth="1"/>
+    <col min="17" max="17" width="20.1640625" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
+      </c>
       <c r="I6" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>15</v>
+        <v>142</v>
       </c>
       <c r="K6" t="s">
+        <v>114</v>
+      </c>
+      <c r="L6" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" t="s">
+        <v>116</v>
+      </c>
+      <c r="O6" t="s">
+        <v>117</v>
+      </c>
+      <c r="P6" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>124</v>
+      </c>
+      <c r="R6" t="s">
+        <v>3</v>
+      </c>
+      <c r="S6" t="s">
+        <v>195</v>
+      </c>
+      <c r="T6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>121</v>
+      </c>
+      <c r="I7" t="s">
+        <v>126</v>
+      </c>
+      <c r="J7" t="s">
+        <v>148</v>
+      </c>
+      <c r="K7" t="s">
+        <v>131</v>
+      </c>
+      <c r="L7" t="s">
+        <v>135</v>
+      </c>
+      <c r="M7">
+        <v>23</v>
+      </c>
+      <c r="N7">
+        <v>60601</v>
+      </c>
+      <c r="O7" t="s">
+        <v>137</v>
+      </c>
+      <c r="P7" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q7">
+        <v>70</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>120</v>
+      </c>
+      <c r="T7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>118</v>
+      </c>
+      <c r="I8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J8" t="s">
+        <v>175</v>
+      </c>
+      <c r="K8" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" t="s">
+        <v>135</v>
+      </c>
+      <c r="M8">
+        <v>24</v>
+      </c>
+      <c r="N8">
+        <v>60601</v>
+      </c>
+      <c r="O8" t="s">
+        <v>138</v>
+      </c>
+      <c r="P8" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q8">
+        <v>70</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>121</v>
+      </c>
+      <c r="T8">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>123</v>
+      </c>
+      <c r="I9" t="s">
+        <v>128</v>
+      </c>
+      <c r="J9" t="s">
+        <v>184</v>
+      </c>
+      <c r="K9" t="s">
+        <v>133</v>
+      </c>
+      <c r="L9" t="s">
+        <v>135</v>
+      </c>
+      <c r="M9">
+        <v>40</v>
+      </c>
+      <c r="N9">
+        <v>60601</v>
+      </c>
+      <c r="O9" t="s">
+        <v>139</v>
+      </c>
+      <c r="P9" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q9">
+        <v>70</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>122</v>
+      </c>
+      <c r="T9">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>125</v>
+      </c>
+      <c r="I10" t="s">
+        <v>129</v>
+      </c>
+      <c r="J10" t="s">
+        <v>174</v>
+      </c>
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" t="s">
+        <v>136</v>
+      </c>
+      <c r="M10">
+        <v>79</v>
+      </c>
+      <c r="N10">
+        <v>60601</v>
+      </c>
+      <c r="O10" t="s">
+        <v>139</v>
+      </c>
+      <c r="P10" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q10">
+        <v>70</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>123</v>
+      </c>
+      <c r="T10">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>192</v>
+      </c>
+      <c r="I11" t="s">
+        <v>130</v>
+      </c>
+      <c r="J11" t="s">
+        <v>175</v>
+      </c>
+      <c r="K11" t="s">
+        <v>134</v>
+      </c>
+      <c r="L11" t="s">
+        <v>136</v>
+      </c>
+      <c r="M11">
+        <v>80</v>
+      </c>
+      <c r="N11">
+        <v>60601</v>
+      </c>
+      <c r="O11" t="s">
+        <v>139</v>
+      </c>
+      <c r="P11" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q11">
+        <v>70</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>124</v>
+      </c>
+      <c r="T11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="L6" t="s">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" t="s">
-        <v>29</v>
-      </c>
-      <c r="L8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>177</v>
-      </c>
-      <c r="I9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" t="s">
-        <v>90</v>
-      </c>
-      <c r="K10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K11" t="s">
-        <v>31</v>
-      </c>
-      <c r="L11" t="s">
-        <v>30</v>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2158,27 +2688,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9772A3FD-BEF1-40F4-9572-5D20CC2045A5}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="46.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" customWidth="1"/>
-    <col min="13" max="13" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" customWidth="1"/>
+    <col min="13" max="13" width="69.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -2192,7 +2722,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2209,7 +2739,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -2223,7 +2753,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2234,7 +2764,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>180</v>
       </c>
@@ -2242,7 +2772,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>181</v>
       </c>
@@ -2265,7 +2795,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>182</v>
       </c>
@@ -2288,7 +2818,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I8" t="s">
         <v>44</v>
       </c>
@@ -2305,7 +2835,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="I9" t="s">
         <v>45</v>
       </c>
@@ -2322,7 +2852,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I10" t="s">
         <v>46</v>
       </c>
@@ -2339,7 +2869,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>176</v>
       </c>
@@ -2359,7 +2889,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I12" t="s">
         <v>48</v>
       </c>
@@ -2376,7 +2906,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I13" t="s">
         <v>49</v>
       </c>
@@ -2393,7 +2923,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I14" t="s">
         <v>50</v>
       </c>
@@ -2410,7 +2940,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I15" t="s">
         <v>51</v>
       </c>
@@ -2427,7 +2957,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I16" t="s">
         <v>52</v>
       </c>
@@ -2444,7 +2974,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I17" t="s">
         <v>53</v>
       </c>
@@ -2461,7 +2991,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I18" t="s">
         <v>54</v>
       </c>
@@ -2478,7 +3008,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I19" t="s">
         <v>55</v>
       </c>
@@ -2495,7 +3025,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I20" t="s">
         <v>56</v>
       </c>
@@ -2512,7 +3042,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I21" t="s">
         <v>57</v>
       </c>
@@ -2529,7 +3059,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I22" t="s">
         <v>58</v>
       </c>
@@ -2546,7 +3076,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I23" t="s">
         <v>59</v>
       </c>
@@ -2563,7 +3093,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I24" t="s">
         <v>60</v>
       </c>
@@ -2580,7 +3110,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I25" t="s">
         <v>61</v>
       </c>
@@ -2597,7 +3127,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I26" t="s">
         <v>62</v>
       </c>
@@ -2614,7 +3144,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I27" t="s">
         <v>83</v>
       </c>
@@ -2631,7 +3161,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I28" t="s">
         <v>84</v>
       </c>
@@ -2648,7 +3178,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I29" t="s">
         <v>85</v>
       </c>
@@ -2665,7 +3195,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I30" t="s">
         <v>86</v>
       </c>
@@ -2682,7 +3212,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I31" t="s">
         <v>87</v>
       </c>
@@ -2699,7 +3229,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I32" t="s">
         <v>88</v>
       </c>
@@ -2716,7 +3246,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I33" t="s">
         <v>89</v>
       </c>
@@ -2733,7 +3263,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I34" t="s">
         <v>97</v>
       </c>
@@ -2750,7 +3280,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I35" t="s">
         <v>98</v>
       </c>
@@ -2767,7 +3297,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I36" t="s">
         <v>99</v>
       </c>
@@ -2784,7 +3314,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I37" t="s">
         <v>100</v>
       </c>
@@ -2801,7 +3331,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I38" t="s">
         <v>101</v>
       </c>
@@ -2828,252 +3358,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1D7C2F-E788-483F-92A0-7A826F78507E}">
-  <dimension ref="A1:M13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" customWidth="1"/>
-    <col min="12" max="13" width="20.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>218</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>221</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" t="s">
-        <v>209</v>
-      </c>
-      <c r="L7" t="s">
-        <v>219</v>
-      </c>
-      <c r="M7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I8" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="K8" t="s">
-        <v>131</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <v>12345679</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I9" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="K9" t="s">
-        <v>213</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>12345679</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I10" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="K10" t="s">
-        <v>214</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>12345679</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I11" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="K11" t="s">
-        <v>215</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>12345679</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>237</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="K12" t="s">
-        <v>216</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>12345679</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I13" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="K13" t="s">
-        <v>217</v>
-      </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
-      <c r="M13">
-        <v>12345679</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D2BEAD-878D-4C61-B4B1-129D00085AAC}">
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.1640625" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>197</v>
       </c>
@@ -3087,7 +3392,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>185</v>
       </c>
@@ -3101,7 +3406,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>199</v>
       </c>
@@ -3136,7 +3441,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>200</v>
       </c>
@@ -3171,7 +3476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>201</v>
       </c>
@@ -3206,7 +3511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>202</v>
       </c>
@@ -3241,7 +3546,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>203</v>
       </c>
@@ -3276,7 +3581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I8">
         <v>5</v>
       </c>
@@ -3302,7 +3607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>238</v>
       </c>
@@ -3311,306 +3616,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DB1A5A-DDCB-4891-AFE3-44BA495796A4}">
-  <dimension ref="A1:M16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" customWidth="1"/>
-    <col min="17" max="17" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>185</v>
-      </c>
-      <c r="B4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>209</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>227</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>208</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>231</v>
-      </c>
-      <c r="G7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>185</v>
-      </c>
-      <c r="J7" t="s">
-        <v>209</v>
-      </c>
-      <c r="K7" t="s">
-        <v>227</v>
-      </c>
-      <c r="L7" t="s">
-        <v>208</v>
-      </c>
-      <c r="M7" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>228</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>232</v>
-      </c>
-      <c r="G8" t="s">
-        <v>168</v>
-      </c>
-      <c r="H8" t="s">
-        <v>126</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="K8">
-        <v>24</v>
-      </c>
-      <c r="L8">
-        <v>100</v>
-      </c>
-      <c r="M8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>226</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>235</v>
-      </c>
-      <c r="G9" t="s">
-        <v>169</v>
-      </c>
-      <c r="H9" t="s">
-        <v>126</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="K9">
-        <v>25</v>
-      </c>
-      <c r="L9">
-        <v>130</v>
-      </c>
-      <c r="M9">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G10" t="s">
-        <v>170</v>
-      </c>
-      <c r="H10" t="s">
-        <v>127</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="K10">
-        <v>36</v>
-      </c>
-      <c r="L10">
-        <v>140</v>
-      </c>
-      <c r="M10">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G11" t="s">
-        <v>171</v>
-      </c>
-      <c r="H11" t="s">
-        <v>128</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="K11">
-        <v>27</v>
-      </c>
-      <c r="L11">
-        <v>146</v>
-      </c>
-      <c r="M11">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G12" t="s">
-        <v>172</v>
-      </c>
-      <c r="H12" t="s">
-        <v>128</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="K12">
-        <v>48</v>
-      </c>
-      <c r="L12">
-        <v>200</v>
-      </c>
-      <c r="M12">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G13" t="s">
-        <v>173</v>
-      </c>
-      <c r="H13" t="s">
-        <v>128</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>190</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3623,72 +3628,72 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>242</v>
       </c>

</xml_diff>